<commit_message>
update template and output
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cm1djm\Documents\GitLab Projects\SPECTRUM\Projects\smoke free dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D99BF5B-0471-4464-8638-765A2FC6DCD0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C398DBA-52C9-41FC-8BCE-706523330375}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="689" activeTab="1" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="689" activeTab="3" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Inequalities" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
   <si>
     <t>Table 2. Average weekly spend on tobacco by socio-economic status (SES) and age group</t>
   </si>
@@ -146,14 +146,24 @@
   </si>
   <si>
     <t>Total Estimated Annual Expenditure (£000,000s)</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>Female</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -254,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -281,6 +291,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -629,11 +640,11 @@
   </sheetPr>
   <dimension ref="A1:N464"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="K230" sqref="K230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -651,21 +662,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="12" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="13"/>
+      <c r="G1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -716,716 +727,946 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E3" s="11"/>
+      <c r="K3" s="12"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E4" s="11"/>
+      <c r="K4" s="12"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E5" s="11"/>
+      <c r="K5" s="12"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E6" s="11"/>
+      <c r="K6" s="12"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E7" s="11"/>
+      <c r="K7" s="12"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E8" s="11"/>
+      <c r="K8" s="12"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E9" s="11"/>
+      <c r="K9" s="12"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E10" s="11"/>
+      <c r="K10" s="12"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E11" s="11"/>
+      <c r="K11" s="12"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E12" s="11"/>
+      <c r="K12" s="12"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E13" s="11"/>
+      <c r="K13" s="12"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E14" s="11"/>
+      <c r="K14" s="12"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E15" s="11"/>
+      <c r="K15" s="12"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="E16" s="11"/>
-    </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K16" s="12"/>
+    </row>
+    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K17" s="12"/>
+    </row>
+    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K18" s="12"/>
+    </row>
+    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K19" s="12"/>
+    </row>
+    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K20" s="12"/>
+    </row>
+    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K21" s="12"/>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E22" s="11"/>
-    </row>
-    <row r="23" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K22" s="12"/>
+    </row>
+    <row r="23" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E24" s="11"/>
-    </row>
-    <row r="25" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E25" s="11"/>
-    </row>
-    <row r="26" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E27" s="11"/>
-    </row>
-    <row r="28" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E28" s="11"/>
-    </row>
-    <row r="29" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E29" s="11"/>
-    </row>
-    <row r="30" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E30" s="11"/>
-    </row>
-    <row r="31" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K30" s="12"/>
+    </row>
+    <row r="31" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E31" s="11"/>
-    </row>
-    <row r="32" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K31" s="12"/>
+    </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K33" s="12"/>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E34" s="11"/>
-    </row>
-    <row r="35" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K34" s="12"/>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E36" s="11"/>
-    </row>
-    <row r="37" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E37" s="11"/>
-    </row>
-    <row r="38" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K37" s="12"/>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K38" s="12"/>
+    </row>
+    <row r="39" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E39" s="11"/>
-    </row>
-    <row r="40" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K39" s="12"/>
+    </row>
+    <row r="40" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E40" s="11"/>
-    </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K40" s="12"/>
+    </row>
+    <row r="41" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K41" s="12"/>
+    </row>
+    <row r="42" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E42" s="11"/>
-    </row>
-    <row r="43" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K42" s="12"/>
+    </row>
+    <row r="43" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E43" s="11"/>
-    </row>
-    <row r="44" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K43" s="12"/>
+    </row>
+    <row r="44" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E44" s="11"/>
-    </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K44" s="12"/>
+    </row>
+    <row r="45" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E45" s="11"/>
-    </row>
-    <row r="46" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K45" s="12"/>
+    </row>
+    <row r="46" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E46" s="11"/>
-    </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K46" s="12"/>
+    </row>
+    <row r="47" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E47" s="11"/>
-    </row>
-    <row r="48" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K47" s="12"/>
+    </row>
+    <row r="48" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E48" s="11"/>
-    </row>
-    <row r="49" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K48" s="12"/>
+    </row>
+    <row r="49" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E49" s="11"/>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K49" s="12"/>
+    </row>
+    <row r="50" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E50" s="11"/>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K50" s="12"/>
+    </row>
+    <row r="51" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E51" s="11"/>
-    </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E52" s="11"/>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K52" s="12"/>
+    </row>
+    <row r="53" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E53" s="11"/>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E54" s="11"/>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E55" s="11"/>
-    </row>
-    <row r="56" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E56" s="11"/>
-    </row>
-    <row r="57" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E57" s="11"/>
-    </row>
-    <row r="58" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K57" s="12"/>
+    </row>
+    <row r="58" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E58" s="11"/>
-    </row>
-    <row r="59" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K58" s="12"/>
+    </row>
+    <row r="59" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E59" s="11"/>
-    </row>
-    <row r="60" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E60" s="11"/>
-    </row>
-    <row r="61" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E61" s="11"/>
-    </row>
-    <row r="62" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K61" s="12"/>
+    </row>
+    <row r="62" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E62" s="11"/>
-    </row>
-    <row r="63" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E63" s="11"/>
-    </row>
-    <row r="64" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K63" s="12"/>
+    </row>
+    <row r="64" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E64" s="11"/>
-    </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K64" s="12"/>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E65" s="11"/>
-    </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K65" s="12"/>
+    </row>
+    <row r="66" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E66" s="11"/>
-    </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K66" s="12"/>
+    </row>
+    <row r="67" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E67" s="11"/>
-    </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K67" s="12"/>
+    </row>
+    <row r="68" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E68" s="11"/>
-    </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K68" s="12"/>
+    </row>
+    <row r="69" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E69" s="11"/>
-    </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K69" s="12"/>
+    </row>
+    <row r="70" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E70" s="11"/>
-    </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K70" s="12"/>
+    </row>
+    <row r="71" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E71" s="11"/>
-    </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K71" s="12"/>
+    </row>
+    <row r="72" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E72" s="11"/>
-    </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K72" s="12"/>
+    </row>
+    <row r="73" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E73" s="11"/>
-    </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K73" s="12"/>
+    </row>
+    <row r="74" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E74" s="11"/>
-    </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K74" s="12"/>
+    </row>
+    <row r="75" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E75" s="11"/>
-    </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K75" s="12"/>
+    </row>
+    <row r="76" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E76" s="11"/>
-    </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K76" s="12"/>
+    </row>
+    <row r="77" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E77" s="11"/>
-    </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K77" s="12"/>
+    </row>
+    <row r="78" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E78" s="11"/>
-    </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K78" s="12"/>
+    </row>
+    <row r="79" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E79" s="11"/>
-    </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K79" s="12"/>
+    </row>
+    <row r="80" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E80" s="11"/>
-    </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K80" s="12"/>
+    </row>
+    <row r="81" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E81" s="11"/>
-    </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K81" s="12"/>
+    </row>
+    <row r="82" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E82" s="11"/>
-    </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K82" s="12"/>
+    </row>
+    <row r="83" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E83" s="11"/>
-    </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K83" s="12"/>
+    </row>
+    <row r="84" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E84" s="11"/>
-    </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K84" s="12"/>
+    </row>
+    <row r="85" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E85" s="11"/>
-    </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K85" s="12"/>
+    </row>
+    <row r="86" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E86" s="11"/>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K86" s="12"/>
+    </row>
+    <row r="87" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E87" s="11"/>
-    </row>
-    <row r="88" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K87" s="12"/>
+    </row>
+    <row r="88" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E88" s="11"/>
-    </row>
-    <row r="89" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K88" s="12"/>
+    </row>
+    <row r="89" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E89" s="11"/>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K89" s="12"/>
+    </row>
+    <row r="90" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E90" s="11"/>
-    </row>
-    <row r="91" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K90" s="12"/>
+    </row>
+    <row r="91" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E91" s="11"/>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K91" s="12"/>
+    </row>
+    <row r="92" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E92" s="11"/>
-    </row>
-    <row r="93" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K92" s="12"/>
+    </row>
+    <row r="93" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E93" s="11"/>
-    </row>
-    <row r="94" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K93" s="12"/>
+    </row>
+    <row r="94" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E94" s="11"/>
-    </row>
-    <row r="95" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K94" s="12"/>
+    </row>
+    <row r="95" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E95" s="11"/>
-    </row>
-    <row r="96" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K95" s="12"/>
+    </row>
+    <row r="96" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E96" s="11"/>
-    </row>
-    <row r="97" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K96" s="12"/>
+    </row>
+    <row r="97" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E97" s="11"/>
-    </row>
-    <row r="98" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K97" s="12"/>
+    </row>
+    <row r="98" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E98" s="11"/>
-    </row>
-    <row r="99" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K98" s="12"/>
+    </row>
+    <row r="99" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E99" s="11"/>
-    </row>
-    <row r="100" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K99" s="12"/>
+    </row>
+    <row r="100" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E100" s="11"/>
-    </row>
-    <row r="101" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K100" s="12"/>
+    </row>
+    <row r="101" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E101" s="11"/>
-    </row>
-    <row r="102" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K101" s="12"/>
+    </row>
+    <row r="102" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E102" s="11"/>
-    </row>
-    <row r="103" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K102" s="12"/>
+    </row>
+    <row r="103" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E103" s="11"/>
-    </row>
-    <row r="104" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K103" s="12"/>
+    </row>
+    <row r="104" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E104" s="11"/>
-    </row>
-    <row r="105" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K104" s="12"/>
+    </row>
+    <row r="105" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E105" s="11"/>
-    </row>
-    <row r="106" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K105" s="12"/>
+    </row>
+    <row r="106" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E106" s="11"/>
-    </row>
-    <row r="107" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K106" s="12"/>
+    </row>
+    <row r="107" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E107" s="11"/>
-    </row>
-    <row r="108" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K107" s="12"/>
+    </row>
+    <row r="108" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E108" s="11"/>
-    </row>
-    <row r="109" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K108" s="12"/>
+    </row>
+    <row r="109" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E109" s="11"/>
-    </row>
-    <row r="110" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K109" s="12"/>
+    </row>
+    <row r="110" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E110" s="11"/>
-    </row>
-    <row r="111" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K110" s="12"/>
+    </row>
+    <row r="111" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E111" s="11"/>
-    </row>
-    <row r="112" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K111" s="12"/>
+    </row>
+    <row r="112" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E112" s="11"/>
-    </row>
-    <row r="113" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K112" s="12"/>
+    </row>
+    <row r="113" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E113" s="11"/>
-    </row>
-    <row r="114" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K113" s="12"/>
+    </row>
+    <row r="114" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E114" s="11"/>
-    </row>
-    <row r="115" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K114" s="12"/>
+    </row>
+    <row r="115" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E115" s="11"/>
-    </row>
-    <row r="116" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K115" s="12"/>
+    </row>
+    <row r="116" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E116" s="11"/>
-    </row>
-    <row r="117" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K116" s="12"/>
+    </row>
+    <row r="117" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E117" s="11"/>
-    </row>
-    <row r="118" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K117" s="12"/>
+    </row>
+    <row r="118" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E118" s="11"/>
-    </row>
-    <row r="119" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K118" s="12"/>
+    </row>
+    <row r="119" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E119" s="11"/>
-    </row>
-    <row r="120" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K119" s="12"/>
+    </row>
+    <row r="120" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E120" s="11"/>
-    </row>
-    <row r="121" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K120" s="12"/>
+    </row>
+    <row r="121" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E121" s="11"/>
-    </row>
-    <row r="122" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K121" s="12"/>
+    </row>
+    <row r="122" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E122" s="11"/>
-    </row>
-    <row r="123" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K122" s="12"/>
+    </row>
+    <row r="123" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E123" s="11"/>
-    </row>
-    <row r="124" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K123" s="12"/>
+    </row>
+    <row r="124" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E124" s="11"/>
-    </row>
-    <row r="125" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K124" s="12"/>
+    </row>
+    <row r="125" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E125" s="11"/>
-    </row>
-    <row r="126" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K125" s="12"/>
+    </row>
+    <row r="126" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E126" s="11"/>
-    </row>
-    <row r="127" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K126" s="12"/>
+    </row>
+    <row r="127" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E127" s="11"/>
-    </row>
-    <row r="128" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K127" s="12"/>
+    </row>
+    <row r="128" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E128" s="11"/>
-    </row>
-    <row r="129" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K128" s="12"/>
+    </row>
+    <row r="129" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E129" s="11"/>
-    </row>
-    <row r="130" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K129" s="12"/>
+    </row>
+    <row r="130" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E130" s="11"/>
-    </row>
-    <row r="131" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K130" s="12"/>
+    </row>
+    <row r="131" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E131" s="11"/>
-    </row>
-    <row r="132" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K131" s="12"/>
+    </row>
+    <row r="132" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E132" s="11"/>
-    </row>
-    <row r="133" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K132" s="12"/>
+    </row>
+    <row r="133" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E133" s="11"/>
-    </row>
-    <row r="134" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K133" s="12"/>
+    </row>
+    <row r="134" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E134" s="11"/>
-    </row>
-    <row r="135" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K134" s="12"/>
+    </row>
+    <row r="135" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E135" s="11"/>
-    </row>
-    <row r="136" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K135" s="12"/>
+    </row>
+    <row r="136" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E136" s="11"/>
-    </row>
-    <row r="137" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K136" s="12"/>
+    </row>
+    <row r="137" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E137" s="11"/>
-    </row>
-    <row r="138" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K137" s="12"/>
+    </row>
+    <row r="138" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E138" s="11"/>
-    </row>
-    <row r="139" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K138" s="12"/>
+    </row>
+    <row r="139" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E139" s="11"/>
-    </row>
-    <row r="140" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K139" s="12"/>
+    </row>
+    <row r="140" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E140" s="11"/>
-    </row>
-    <row r="141" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K140" s="12"/>
+    </row>
+    <row r="141" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E141" s="11"/>
-    </row>
-    <row r="142" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K141" s="12"/>
+    </row>
+    <row r="142" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E142" s="11"/>
-    </row>
-    <row r="143" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K142" s="12"/>
+    </row>
+    <row r="143" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E143" s="11"/>
-    </row>
-    <row r="144" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K143" s="12"/>
+    </row>
+    <row r="144" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E144" s="11"/>
-    </row>
-    <row r="145" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K144" s="12"/>
+    </row>
+    <row r="145" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E145" s="11"/>
-    </row>
-    <row r="146" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K145" s="12"/>
+    </row>
+    <row r="146" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E146" s="11"/>
-    </row>
-    <row r="147" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K146" s="12"/>
+    </row>
+    <row r="147" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E147" s="11"/>
-    </row>
-    <row r="148" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K147" s="12"/>
+    </row>
+    <row r="148" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E148" s="11"/>
-    </row>
-    <row r="149" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K148" s="12"/>
+    </row>
+    <row r="149" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E149" s="11"/>
-    </row>
-    <row r="150" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K149" s="12"/>
+    </row>
+    <row r="150" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E150" s="11"/>
-    </row>
-    <row r="151" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K150" s="12"/>
+    </row>
+    <row r="151" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E151" s="11"/>
-    </row>
-    <row r="152" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K151" s="12"/>
+    </row>
+    <row r="152" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E152" s="11"/>
-    </row>
-    <row r="153" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K152" s="12"/>
+    </row>
+    <row r="153" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E153" s="11"/>
-    </row>
-    <row r="154" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K153" s="12"/>
+    </row>
+    <row r="154" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E154" s="11"/>
-    </row>
-    <row r="155" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K154" s="12"/>
+    </row>
+    <row r="155" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E155" s="11"/>
-    </row>
-    <row r="156" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K155" s="12"/>
+    </row>
+    <row r="156" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E156" s="11"/>
-    </row>
-    <row r="157" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K156" s="12"/>
+    </row>
+    <row r="157" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E157" s="11"/>
-    </row>
-    <row r="158" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K157" s="12"/>
+    </row>
+    <row r="158" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E158" s="11"/>
-    </row>
-    <row r="159" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K158" s="12"/>
+    </row>
+    <row r="159" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E159" s="11"/>
-    </row>
-    <row r="160" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K159" s="12"/>
+    </row>
+    <row r="160" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E160" s="11"/>
-    </row>
-    <row r="161" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K160" s="12"/>
+    </row>
+    <row r="161" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E161" s="11"/>
-    </row>
-    <row r="162" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K161" s="12"/>
+    </row>
+    <row r="162" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E162" s="11"/>
-    </row>
-    <row r="163" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K162" s="12"/>
+    </row>
+    <row r="163" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E163" s="11"/>
-    </row>
-    <row r="164" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K163" s="12"/>
+    </row>
+    <row r="164" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E164" s="11"/>
-    </row>
-    <row r="165" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K164" s="12"/>
+    </row>
+    <row r="165" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E165" s="11"/>
-    </row>
-    <row r="166" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K165" s="12"/>
+    </row>
+    <row r="166" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E166" s="11"/>
-    </row>
-    <row r="167" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K166" s="12"/>
+    </row>
+    <row r="167" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E167" s="11"/>
-    </row>
-    <row r="168" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K167" s="12"/>
+    </row>
+    <row r="168" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E168" s="11"/>
-    </row>
-    <row r="169" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K168" s="12"/>
+    </row>
+    <row r="169" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E169" s="11"/>
-    </row>
-    <row r="170" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K169" s="12"/>
+    </row>
+    <row r="170" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E170" s="11"/>
-    </row>
-    <row r="171" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K170" s="12"/>
+    </row>
+    <row r="171" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E171" s="11"/>
-    </row>
-    <row r="172" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K171" s="12"/>
+    </row>
+    <row r="172" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E172" s="11"/>
-    </row>
-    <row r="173" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K172" s="12"/>
+    </row>
+    <row r="173" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E173" s="11"/>
-    </row>
-    <row r="174" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K173" s="12"/>
+    </row>
+    <row r="174" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E174" s="11"/>
-    </row>
-    <row r="175" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K174" s="12"/>
+    </row>
+    <row r="175" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E175" s="11"/>
-    </row>
-    <row r="176" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K175" s="12"/>
+    </row>
+    <row r="176" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E176" s="11"/>
-    </row>
-    <row r="177" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K176" s="12"/>
+    </row>
+    <row r="177" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E177" s="11"/>
-    </row>
-    <row r="178" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K177" s="12"/>
+    </row>
+    <row r="178" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E178" s="11"/>
-    </row>
-    <row r="179" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K178" s="12"/>
+    </row>
+    <row r="179" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E179" s="11"/>
-    </row>
-    <row r="180" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K179" s="12"/>
+    </row>
+    <row r="180" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E180" s="11"/>
-    </row>
-    <row r="181" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K180" s="12"/>
+    </row>
+    <row r="181" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E181" s="11"/>
-    </row>
-    <row r="182" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K181" s="12"/>
+    </row>
+    <row r="182" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E182" s="11"/>
-    </row>
-    <row r="183" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K182" s="12"/>
+    </row>
+    <row r="183" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E183" s="11"/>
-    </row>
-    <row r="184" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K183" s="12"/>
+    </row>
+    <row r="184" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E184" s="11"/>
-    </row>
-    <row r="185" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K184" s="12"/>
+    </row>
+    <row r="185" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E185" s="11"/>
-    </row>
-    <row r="186" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K185" s="12"/>
+    </row>
+    <row r="186" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E186" s="11"/>
-    </row>
-    <row r="187" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K186" s="12"/>
+    </row>
+    <row r="187" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E187" s="11"/>
-    </row>
-    <row r="188" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K187" s="12"/>
+    </row>
+    <row r="188" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E188" s="11"/>
-    </row>
-    <row r="189" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K188" s="12"/>
+    </row>
+    <row r="189" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E189" s="11"/>
-    </row>
-    <row r="190" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K189" s="12"/>
+    </row>
+    <row r="190" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E190" s="11"/>
-    </row>
-    <row r="191" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K190" s="12"/>
+    </row>
+    <row r="191" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E191" s="11"/>
-    </row>
-    <row r="192" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K191" s="12"/>
+    </row>
+    <row r="192" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E192" s="11"/>
-    </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K192" s="12"/>
+    </row>
+    <row r="193" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E193" s="11"/>
-    </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K193" s="12"/>
+    </row>
+    <row r="194" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E194" s="11"/>
-    </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K194" s="12"/>
+    </row>
+    <row r="195" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E195" s="11"/>
-    </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K195" s="12"/>
+    </row>
+    <row r="196" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E196" s="11"/>
-    </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K196" s="12"/>
+    </row>
+    <row r="197" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E197" s="11"/>
-    </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K197" s="12"/>
+    </row>
+    <row r="198" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E198" s="11"/>
-    </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K198" s="12"/>
+    </row>
+    <row r="199" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E199" s="11"/>
-    </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K199" s="12"/>
+    </row>
+    <row r="200" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E200" s="11"/>
-    </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K200" s="12"/>
+    </row>
+    <row r="201" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E201" s="11"/>
-    </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K201" s="12"/>
+    </row>
+    <row r="202" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E202" s="11"/>
-    </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K202" s="12"/>
+    </row>
+    <row r="203" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E203" s="11"/>
-    </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K203" s="12"/>
+    </row>
+    <row r="204" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E204" s="11"/>
-    </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K204" s="12"/>
+    </row>
+    <row r="205" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E205" s="11"/>
-    </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K205" s="12"/>
+    </row>
+    <row r="206" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E206" s="11"/>
-    </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K206" s="12"/>
+    </row>
+    <row r="207" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E207" s="11"/>
-    </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K207" s="12"/>
+    </row>
+    <row r="208" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E208" s="11"/>
-    </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K208" s="12"/>
+    </row>
+    <row r="209" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E209" s="11"/>
-    </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K209" s="12"/>
+    </row>
+    <row r="210" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E210" s="11"/>
-    </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K210" s="12"/>
+    </row>
+    <row r="211" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E211" s="11"/>
-    </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K211" s="12"/>
+    </row>
+    <row r="212" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E212" s="11"/>
-    </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K212" s="12"/>
+    </row>
+    <row r="213" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E213" s="11"/>
-    </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K213" s="12"/>
+    </row>
+    <row r="214" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E214" s="11"/>
-    </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K214" s="12"/>
+    </row>
+    <row r="215" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E215" s="11"/>
-    </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K215" s="12"/>
+    </row>
+    <row r="216" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E216" s="11"/>
-    </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K216" s="12"/>
+    </row>
+    <row r="217" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E217" s="11"/>
-    </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K217" s="12"/>
+    </row>
+    <row r="218" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E218" s="11"/>
-    </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K218" s="12"/>
+    </row>
+    <row r="219" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E219" s="11"/>
-    </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K219" s="12"/>
+    </row>
+    <row r="220" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E220" s="11"/>
-    </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K220" s="12"/>
+    </row>
+    <row r="221" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E221" s="11"/>
-    </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K221" s="12"/>
+    </row>
+    <row r="222" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E222" s="11"/>
-    </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K222" s="12"/>
+    </row>
+    <row r="223" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E223" s="11"/>
-    </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K223" s="12"/>
+    </row>
+    <row r="224" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E224" s="11"/>
-    </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K224" s="12"/>
+    </row>
+    <row r="225" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E225" s="11"/>
-    </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K225" s="12"/>
+    </row>
+    <row r="226" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E226" s="11"/>
-    </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K226" s="12"/>
+    </row>
+    <row r="227" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E227" s="11"/>
-    </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K227" s="12"/>
+    </row>
+    <row r="228" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E228" s="11"/>
-    </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K228" s="12"/>
+    </row>
+    <row r="229" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E229" s="11"/>
-    </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K229" s="12"/>
+    </row>
+    <row r="230" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E230" s="11"/>
-    </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K230" s="12"/>
+    </row>
+    <row r="231" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E231" s="11"/>
-    </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K231" s="12"/>
+    </row>
+    <row r="232" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E232" s="11"/>
-    </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.35">
+      <c r="K232" s="12"/>
+    </row>
+    <row r="233" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E233" s="11"/>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="234" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E234" s="11"/>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="235" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E235" s="11"/>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="236" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E236" s="11"/>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="237" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E237" s="11"/>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="238" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E238" s="11"/>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="239" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E239" s="11"/>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="240" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E240" s="11"/>
     </row>
     <row r="241" spans="5:5" x14ac:dyDescent="0.35">
@@ -2133,10 +2374,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2150,10 +2391,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
@@ -2178,34 +2419,47 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update workflow and results
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Documents\GitLab Projects\SPECTRUM\projects\smoke free dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA607FD0-E6F2-4B9E-BC74-D6384FEAB27E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7EE187-8546-43EC-8FC4-640D414A73B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" firstSheet="3" activeTab="5" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="4" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Inequalities" sheetId="5" r:id="rId1"/>
+    <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
     <sheet name="LA data" sheetId="6" r:id="rId2"/>
-    <sheet name="Upshift Calcs" sheetId="1" r:id="rId3"/>
-    <sheet name="Average Tobacco Spend" sheetId="2" r:id="rId4"/>
-    <sheet name="Expenditure % of Income" sheetId="3" r:id="rId5"/>
-    <sheet name="Expenditure % of Income LA" sheetId="4" r:id="rId6"/>
+    <sheet name="Average Tobacco Spend" sheetId="2" r:id="rId3"/>
+    <sheet name="Expenditure % of Income" sheetId="3" r:id="rId4"/>
+    <sheet name="Expenditure % of Income LA" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
   <si>
     <t>Table 2. Average weekly spend on tobacco by socio-economic status (SES) and age group</t>
   </si>
@@ -79,9 +78,6 @@
     <t>65+</t>
   </si>
   <si>
-    <t>Table 3. Expenditure of smoking as a proportion of income</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -91,9 +87,6 @@
     <t>% of income spent on tobacco</t>
   </si>
   <si>
-    <t>Table 4. Expenditure of smoking in the local authorities with the highest tobacco expenditure as a proportion of income</t>
-  </si>
-  <si>
     <t>LA</t>
   </si>
   <si>
@@ -155,6 +148,66 @@
   </si>
   <si>
     <t>Annual Smokefree Dividend (£m)</t>
+  </si>
+  <si>
+    <t>Table 4. Expenditure on smoking in the local authorities with the highest tobacco expenditure as a proportion of income</t>
+  </si>
+  <si>
+    <t>Table 3. Expenditure on smoking as a proportion of income</t>
+  </si>
+  <si>
+    <t>HMRC Stats</t>
+  </si>
+  <si>
+    <t>Cigarettes</t>
+  </si>
+  <si>
+    <t>Hand-Rolled</t>
+  </si>
+  <si>
+    <t>Ad-Valorem tax</t>
+  </si>
+  <si>
+    <t>Specific duty</t>
+  </si>
+  <si>
+    <t>Total duties (£m)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Total excise per pack</t>
+  </si>
+  <si>
+    <t>Total excise % of price</t>
+  </si>
+  <si>
+    <t>Price per 100g (Dec 2020)</t>
+  </si>
+  <si>
+    <t>Price per 100g (Dec 2018)</t>
+  </si>
+  <si>
+    <t>Price deflator</t>
+  </si>
+  <si>
+    <t>Total cigarette spend (£m)</t>
+  </si>
+  <si>
+    <t>Total HRT spend (£m)</t>
+  </si>
+  <si>
+    <t>Total grossed-up expenditure</t>
+  </si>
+  <si>
+    <t>Upshift Factor:</t>
+  </si>
+  <si>
+    <t>Pack Price (20 cigs)</t>
+  </si>
+  <si>
+    <t>Survey data estimate</t>
   </si>
 </sst>
 </file>
@@ -191,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -252,6 +305,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -265,7 +336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -305,6 +376,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -619,19 +702,135 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A86223D-A241-431A-81F4-D7025CA5F12D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082015AB-C1A0-4686-BF34-96E964A84A05}">
   <sheetPr>
-    <tabColor theme="9" tint="0.39997558519241921"/>
+    <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="B2:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="23.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="20" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="F11" s="21"/>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="21"/>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B13:F13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -646,34 +845,26 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K230" sqref="K230"/>
+      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="33.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" customWidth="1"/>
-    <col min="7" max="8" width="11.140625" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" customWidth="1"/>
-    <col min="10" max="10" width="19.5703125" customWidth="1"/>
-    <col min="11" max="11" width="20.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="3" max="14" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" s="15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="14"/>
       <c r="G1" s="16" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -685,46 +876,46 @@
     </row>
     <row r="2" spans="1:14" s="3" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="E2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="J2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="L2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="8" t="s">
         <v>26</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -2355,23 +2546,6 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{082015AB-C1A0-4686-BF34-96E964A84A05}">
-  <sheetPr>
-    <tabColor theme="7" tint="0.39997558519241921"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41393E51-CA3C-4A23-9C04-919BFB576ADB}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -2379,12 +2553,12 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2398,7 +2572,7 @@
       </c>
       <c r="B2" s="17"/>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2421,15 +2595,15 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2474,7 +2648,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68574BDA-3780-4F30-ACB9-BC66FA2B1114}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -2482,38 +2656,34 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2578,7 +2748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B55ED5B-4EDE-43B1-AA7B-733BBABD30C8}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -2586,38 +2756,34 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="1" max="5" width="25.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="44.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
update template results table and results accordingly
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work Documents\GitLab Projects\SPECTRUM\projects\smoke free dividend\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLab Projects\SPECTRUM\projects\smoke free dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7EE187-8546-43EC-8FC4-640D414A73B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018B5DD0-843F-4B18-91DE-27342C5683F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="4" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <t>Table 2. Average weekly spend on tobacco by socio-economic status (SES) and age group</t>
   </si>
@@ -165,59 +165,102 @@
     <t>Hand-Rolled</t>
   </si>
   <si>
-    <t>Ad-Valorem tax</t>
-  </si>
-  <si>
-    <t>Specific duty</t>
-  </si>
-  <si>
-    <t>Total duties (£m)</t>
-  </si>
-  <si>
-    <t>Total</t>
-  </si>
-  <si>
-    <t>Total excise per pack</t>
-  </si>
-  <si>
-    <t>Total excise % of price</t>
-  </si>
-  <si>
-    <t>Price per 100g (Dec 2020)</t>
-  </si>
-  <si>
-    <t>Price per 100g (Dec 2018)</t>
-  </si>
-  <si>
-    <t>Price deflator</t>
-  </si>
-  <si>
-    <t>Total cigarette spend (£m)</t>
-  </si>
-  <si>
-    <t>Total HRT spend (£m)</t>
-  </si>
-  <si>
     <t>Total grossed-up expenditure</t>
   </si>
   <si>
     <t>Upshift Factor:</t>
   </si>
   <si>
-    <t>Pack Price (20 cigs)</t>
-  </si>
-  <si>
     <t>Survey data estimate</t>
+  </si>
+  <si>
+    <t>(2) Pack Price (20 cigs)</t>
+  </si>
+  <si>
+    <t>(4) Ad-Valorem tax (per pack)</t>
+  </si>
+  <si>
+    <t>(5) Specific duty (per 1000 cigs)</t>
+  </si>
+  <si>
+    <t>(6) Specific duty (per pack)</t>
+  </si>
+  <si>
+    <t>(7) Total excise per pack</t>
+  </si>
+  <si>
+    <t>(8) Total excise % of price</t>
+  </si>
+  <si>
+    <t>(9) Total cigarette spend (£m)</t>
+  </si>
+  <si>
+    <t>(1) Total duty receipts (£m)</t>
+  </si>
+  <si>
+    <t>(2) * (3)</t>
+  </si>
+  <si>
+    <t>(3) Ad-Valorem tax rate</t>
+  </si>
+  <si>
+    <t>(5) / 20</t>
+  </si>
+  <si>
+    <t>(4) + (6)</t>
+  </si>
+  <si>
+    <t>Dataset :</t>
+  </si>
+  <si>
+    <t>(7) / (2)</t>
+  </si>
+  <si>
+    <t>(1) / (8)</t>
+  </si>
+  <si>
+    <t>(2) Price per 100g (Dec 2020)</t>
+  </si>
+  <si>
+    <t>(3) Price deflator</t>
+  </si>
+  <si>
+    <t>(4) Price per 100g (Dec 2018)</t>
+  </si>
+  <si>
+    <t>(5) Specific duty (per kg)</t>
+  </si>
+  <si>
+    <t>(6) Specific duty (per 100g)</t>
+  </si>
+  <si>
+    <t>(7) Total excise % of price</t>
+  </si>
+  <si>
+    <t>(8) Total HRT spend (£m)</t>
+  </si>
+  <si>
+    <t>(5) / 10</t>
+  </si>
+  <si>
+    <t>(6) / (4)</t>
+  </si>
+  <si>
+    <t>(1) / (7)</t>
+  </si>
+  <si>
+    <t>Totals (£m)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#,##0.000"/>
+    <numFmt numFmtId="167" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -336,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -365,6 +408,27 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -377,18 +441,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -706,128 +759,200 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:F17"/>
+  <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="26.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18" t="s">
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="21"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="D5" s="22"/>
+      <c r="E5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="16"/>
+      <c r="E6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="24"/>
+      <c r="E7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="23"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="22"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="23"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" s="31"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="31"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="H13" s="31"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="H16" s="31"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F11" s="21"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="19" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
-      <c r="F13" s="19"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="21"/>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="23" t="s">
-        <v>54</v>
-      </c>
-      <c r="C17" s="22"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="B15:H15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -855,21 +980,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="14" t="s">
+      <c r="D1" s="28"/>
+      <c r="E1" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="14"/>
-      <c r="G1" s="16" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -2567,10 +2692,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="17"/>
+      <c r="B2" s="30"/>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
@@ -2755,7 +2880,7 @@
   </sheetPr>
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
include consumption results in the table template and results
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitLab Projects\SPECTRUM\projects\smoke free dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{018B5DD0-843F-4B18-91DE-27342C5683F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{402E96D9-FD0C-4C5B-BBD5-BDE0819E9F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="2" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
     <sheet name="LA data" sheetId="6" r:id="rId2"/>
-    <sheet name="Average Tobacco Spend" sheetId="2" r:id="rId3"/>
-    <sheet name="Expenditure % of Income" sheetId="3" r:id="rId4"/>
-    <sheet name="Expenditure % of Income LA" sheetId="4" r:id="rId5"/>
+    <sheet name="Consumption" sheetId="7" r:id="rId3"/>
+    <sheet name="Average Tobacco Spend" sheetId="2" r:id="rId4"/>
+    <sheet name="Expenditure % of Income" sheetId="3" r:id="rId5"/>
+    <sheet name="Expenditure % of Income LA" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>Table 2. Average weekly spend on tobacco by socio-economic status (SES) and age group</t>
   </si>
@@ -250,6 +251,30 @@
   </si>
   <si>
     <t>Totals (£m)</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>STS calculated (smokers only)</t>
+  </si>
+  <si>
+    <t>Average Daily Total Cigarettes</t>
+  </si>
+  <si>
+    <t>Average Daily FM Cigarettes</t>
+  </si>
+  <si>
+    <t>Average Daily RYO Cigarettes</t>
+  </si>
+  <si>
+    <t>Average % of Cigs Roll-Your-Own</t>
+  </si>
+  <si>
+    <t>% of Smokers Consume RYO</t>
+  </si>
+  <si>
+    <t>% of Smokers Consume FM</t>
   </si>
 </sst>
 </file>
@@ -367,7 +392,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -375,11 +400,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -423,6 +459,10 @@
     <xf numFmtId="167" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -441,7 +481,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,7 +802,7 @@
   </sheetPr>
   <dimension ref="B2:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -777,27 +818,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="26" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
       <c r="H3" s="14" t="s">
         <v>70</v>
       </c>
@@ -904,7 +945,7 @@
       <c r="F11" t="s">
         <v>69</v>
       </c>
-      <c r="G11" s="31"/>
+      <c r="G11" s="26"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
@@ -913,27 +954,27 @@
       <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="31"/>
+      <c r="D12" s="26"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H13" s="31"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="H16" s="31"/>
+      <c r="H16" s="26"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
@@ -967,10 +1008,10 @@
   <dimension ref="A1:N464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,21 +1021,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="27" t="s">
+      <c r="D1" s="30"/>
+      <c r="E1" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="27"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="29"/>
+      <c r="G1" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
       <c r="L1" s="9"/>
       <c r="M1" s="9"/>
       <c r="N1" s="9"/>
@@ -2671,6 +2712,3738 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54BADBFD-829B-43FA-95E8-F9BEA11B5B6C}">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:H460"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="33.5703125" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="26.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" customWidth="1"/>
+    <col min="6" max="8" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="34"/>
+      <c r="D8" s="34"/>
+      <c r="E8" s="34"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="34"/>
+      <c r="D9" s="34"/>
+      <c r="E9" s="34"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="34"/>
+      <c r="D11" s="34"/>
+      <c r="E11" s="34"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="20"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="20"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="20"/>
+      <c r="H17" s="20"/>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="20"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="34"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="20"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="34"/>
+      <c r="D24" s="34"/>
+      <c r="E24" s="34"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="34"/>
+      <c r="D25" s="34"/>
+      <c r="E25" s="34"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="34"/>
+      <c r="D26" s="34"/>
+      <c r="E26" s="34"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="20"/>
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C33" s="34"/>
+      <c r="D33" s="34"/>
+      <c r="E33" s="34"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C34" s="34"/>
+      <c r="D34" s="34"/>
+      <c r="E34" s="34"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C35" s="34"/>
+      <c r="D35" s="34"/>
+      <c r="E35" s="34"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C36" s="34"/>
+      <c r="D36" s="34"/>
+      <c r="E36" s="34"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="37" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C37" s="34"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+    </row>
+    <row r="38" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C38" s="34"/>
+      <c r="D38" s="34"/>
+      <c r="E38" s="34"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="39" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C39" s="34"/>
+      <c r="D39" s="34"/>
+      <c r="E39" s="34"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C40" s="34"/>
+      <c r="D40" s="34"/>
+      <c r="E40" s="34"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+    </row>
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+    </row>
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="20"/>
+      <c r="H42" s="20"/>
+    </row>
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="20"/>
+      <c r="H43" s="20"/>
+    </row>
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="20"/>
+      <c r="H44" s="20"/>
+    </row>
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+    </row>
+    <row r="46" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="20"/>
+      <c r="H46" s="20"/>
+    </row>
+    <row r="47" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="20"/>
+      <c r="H47" s="20"/>
+    </row>
+    <row r="48" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="20"/>
+      <c r="H48" s="20"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="20"/>
+      <c r="H51" s="20"/>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="20"/>
+      <c r="H52" s="20"/>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="20"/>
+      <c r="H53" s="20"/>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+      <c r="H54" s="20"/>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" s="34"/>
+      <c r="D55" s="34"/>
+      <c r="E55" s="34"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" s="34"/>
+      <c r="D56" s="34"/>
+      <c r="E56" s="34"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="20"/>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57" s="34"/>
+      <c r="D57" s="34"/>
+      <c r="E57" s="34"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="20"/>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58" s="34"/>
+      <c r="D58" s="34"/>
+      <c r="E58" s="34"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="20"/>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59" s="34"/>
+      <c r="D59" s="34"/>
+      <c r="E59" s="34"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="20"/>
+      <c r="H59" s="20"/>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60" s="34"/>
+      <c r="D60" s="34"/>
+      <c r="E60" s="34"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61" s="34"/>
+      <c r="D61" s="34"/>
+      <c r="E61" s="34"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="20"/>
+      <c r="H61" s="20"/>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62" s="34"/>
+      <c r="D62" s="34"/>
+      <c r="E62" s="34"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="20"/>
+      <c r="H62" s="20"/>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C63" s="34"/>
+      <c r="D63" s="34"/>
+      <c r="E63" s="34"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="20"/>
+      <c r="H63" s="20"/>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64" s="34"/>
+      <c r="D64" s="34"/>
+      <c r="E64" s="34"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="20"/>
+      <c r="H64" s="20"/>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65" s="34"/>
+      <c r="D65" s="34"/>
+      <c r="E65" s="34"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="20"/>
+      <c r="H65" s="20"/>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66" s="34"/>
+      <c r="D66" s="34"/>
+      <c r="E66" s="34"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="20"/>
+      <c r="H66" s="20"/>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" s="34"/>
+      <c r="D67" s="34"/>
+      <c r="E67" s="34"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="20"/>
+      <c r="H67" s="20"/>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" s="34"/>
+      <c r="D68" s="34"/>
+      <c r="E68" s="34"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="20"/>
+      <c r="H68" s="20"/>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" s="34"/>
+      <c r="D69" s="34"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+      <c r="H69" s="20"/>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" s="34"/>
+      <c r="D70" s="34"/>
+      <c r="E70" s="34"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+      <c r="H70" s="20"/>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" s="34"/>
+      <c r="D71" s="34"/>
+      <c r="E71" s="34"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+      <c r="H71" s="20"/>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" s="34"/>
+      <c r="D72" s="34"/>
+      <c r="E72" s="34"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="20"/>
+      <c r="H72" s="20"/>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73" s="34"/>
+      <c r="D73" s="34"/>
+      <c r="E73" s="34"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="20"/>
+      <c r="H73" s="20"/>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" s="34"/>
+      <c r="D74" s="34"/>
+      <c r="E74" s="34"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="20"/>
+      <c r="H74" s="20"/>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" s="34"/>
+      <c r="D75" s="34"/>
+      <c r="E75" s="34"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20"/>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="20"/>
+      <c r="H76" s="20"/>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77" s="34"/>
+      <c r="D77" s="34"/>
+      <c r="E77" s="34"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="20"/>
+      <c r="H77" s="20"/>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C78" s="34"/>
+      <c r="D78" s="34"/>
+      <c r="E78" s="34"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="20"/>
+      <c r="H78" s="20"/>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C79" s="34"/>
+      <c r="D79" s="34"/>
+      <c r="E79" s="34"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="20"/>
+      <c r="H79" s="20"/>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" s="34"/>
+      <c r="D80" s="34"/>
+      <c r="E80" s="34"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="20"/>
+      <c r="H80" s="20"/>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C81" s="34"/>
+      <c r="D81" s="34"/>
+      <c r="E81" s="34"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="20"/>
+      <c r="H81" s="20"/>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C82" s="34"/>
+      <c r="D82" s="34"/>
+      <c r="E82" s="34"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="20"/>
+      <c r="H82" s="20"/>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C83" s="34"/>
+      <c r="D83" s="34"/>
+      <c r="E83" s="34"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="20"/>
+      <c r="H83" s="20"/>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C84" s="34"/>
+      <c r="D84" s="34"/>
+      <c r="E84" s="34"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="20"/>
+      <c r="H84" s="20"/>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C85" s="34"/>
+      <c r="D85" s="34"/>
+      <c r="E85" s="34"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="20"/>
+      <c r="H85" s="20"/>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C86" s="34"/>
+      <c r="D86" s="34"/>
+      <c r="E86" s="34"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="20"/>
+      <c r="H86" s="20"/>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C87" s="34"/>
+      <c r="D87" s="34"/>
+      <c r="E87" s="34"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="20"/>
+      <c r="H87" s="20"/>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="34"/>
+      <c r="D88" s="34"/>
+      <c r="E88" s="34"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="20"/>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C89" s="34"/>
+      <c r="D89" s="34"/>
+      <c r="E89" s="34"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="20"/>
+      <c r="H89" s="20"/>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C91" s="34"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="34"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="20"/>
+      <c r="H91" s="20"/>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C92" s="34"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="20"/>
+      <c r="H92" s="20"/>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="20"/>
+      <c r="H93" s="20"/>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C94" s="34"/>
+      <c r="D94" s="34"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="20"/>
+      <c r="H94" s="20"/>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="20"/>
+      <c r="H95" s="20"/>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C96" s="34"/>
+      <c r="D96" s="34"/>
+      <c r="E96" s="34"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="20"/>
+      <c r="H96" s="20"/>
+    </row>
+    <row r="97" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C97" s="34"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="34"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="20"/>
+      <c r="H97" s="20"/>
+    </row>
+    <row r="98" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="20"/>
+      <c r="H98" s="20"/>
+    </row>
+    <row r="99" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C99" s="34"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="34"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="20"/>
+      <c r="H99" s="20"/>
+    </row>
+    <row r="100" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C100" s="34"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="34"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="20"/>
+      <c r="H100" s="20"/>
+    </row>
+    <row r="101" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C101" s="34"/>
+      <c r="D101" s="34"/>
+      <c r="E101" s="34"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="20"/>
+      <c r="H101" s="20"/>
+    </row>
+    <row r="102" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C102" s="34"/>
+      <c r="D102" s="34"/>
+      <c r="E102" s="34"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="20"/>
+      <c r="H102" s="20"/>
+    </row>
+    <row r="103" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C103" s="34"/>
+      <c r="D103" s="34"/>
+      <c r="E103" s="34"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="20"/>
+      <c r="H103" s="20"/>
+    </row>
+    <row r="104" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C104" s="34"/>
+      <c r="D104" s="34"/>
+      <c r="E104" s="34"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+    </row>
+    <row r="105" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C105" s="34"/>
+      <c r="D105" s="34"/>
+      <c r="E105" s="34"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
+    </row>
+    <row r="106" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C106" s="34"/>
+      <c r="D106" s="34"/>
+      <c r="E106" s="34"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="20"/>
+      <c r="H106" s="20"/>
+    </row>
+    <row r="107" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C107" s="34"/>
+      <c r="D107" s="34"/>
+      <c r="E107" s="34"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="20"/>
+    </row>
+    <row r="108" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C108" s="34"/>
+      <c r="D108" s="34"/>
+      <c r="E108" s="34"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C109" s="34"/>
+      <c r="D109" s="34"/>
+      <c r="E109" s="34"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="20"/>
+      <c r="H109" s="20"/>
+    </row>
+    <row r="110" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C110" s="34"/>
+      <c r="D110" s="34"/>
+      <c r="E110" s="34"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="20"/>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C111" s="34"/>
+      <c r="D111" s="34"/>
+      <c r="E111" s="34"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="20"/>
+      <c r="H111" s="20"/>
+    </row>
+    <row r="112" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C112" s="34"/>
+      <c r="D112" s="34"/>
+      <c r="E112" s="34"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="20"/>
+    </row>
+    <row r="113" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C113" s="34"/>
+      <c r="D113" s="34"/>
+      <c r="E113" s="34"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="20"/>
+    </row>
+    <row r="114" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C114" s="34"/>
+      <c r="D114" s="34"/>
+      <c r="E114" s="34"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="20"/>
+    </row>
+    <row r="115" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C115" s="34"/>
+      <c r="D115" s="34"/>
+      <c r="E115" s="34"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="20"/>
+      <c r="H115" s="20"/>
+    </row>
+    <row r="116" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C116" s="34"/>
+      <c r="D116" s="34"/>
+      <c r="E116" s="34"/>
+      <c r="F116" s="20"/>
+      <c r="G116" s="20"/>
+      <c r="H116" s="20"/>
+    </row>
+    <row r="117" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C117" s="34"/>
+      <c r="D117" s="34"/>
+      <c r="E117" s="34"/>
+      <c r="F117" s="20"/>
+      <c r="G117" s="20"/>
+      <c r="H117" s="20"/>
+    </row>
+    <row r="118" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C118" s="34"/>
+      <c r="D118" s="34"/>
+      <c r="E118" s="34"/>
+      <c r="F118" s="20"/>
+      <c r="G118" s="20"/>
+      <c r="H118" s="20"/>
+    </row>
+    <row r="119" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C119" s="34"/>
+      <c r="D119" s="34"/>
+      <c r="E119" s="34"/>
+      <c r="F119" s="20"/>
+      <c r="G119" s="20"/>
+      <c r="H119" s="20"/>
+    </row>
+    <row r="120" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C120" s="34"/>
+      <c r="D120" s="34"/>
+      <c r="E120" s="34"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
+    </row>
+    <row r="121" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C121" s="34"/>
+      <c r="D121" s="34"/>
+      <c r="E121" s="34"/>
+      <c r="F121" s="20"/>
+      <c r="G121" s="20"/>
+      <c r="H121" s="20"/>
+    </row>
+    <row r="122" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C122" s="34"/>
+      <c r="D122" s="34"/>
+      <c r="E122" s="34"/>
+      <c r="F122" s="20"/>
+      <c r="G122" s="20"/>
+      <c r="H122" s="20"/>
+    </row>
+    <row r="123" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C123" s="34"/>
+      <c r="D123" s="34"/>
+      <c r="E123" s="34"/>
+      <c r="F123" s="20"/>
+      <c r="G123" s="20"/>
+      <c r="H123" s="20"/>
+    </row>
+    <row r="124" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C124" s="34"/>
+      <c r="D124" s="34"/>
+      <c r="E124" s="34"/>
+      <c r="F124" s="20"/>
+      <c r="G124" s="20"/>
+      <c r="H124" s="20"/>
+    </row>
+    <row r="125" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C125" s="34"/>
+      <c r="D125" s="34"/>
+      <c r="E125" s="34"/>
+      <c r="F125" s="20"/>
+      <c r="G125" s="20"/>
+      <c r="H125" s="20"/>
+    </row>
+    <row r="126" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C126" s="34"/>
+      <c r="D126" s="34"/>
+      <c r="E126" s="34"/>
+      <c r="F126" s="20"/>
+      <c r="G126" s="20"/>
+      <c r="H126" s="20"/>
+    </row>
+    <row r="127" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C127" s="34"/>
+      <c r="D127" s="34"/>
+      <c r="E127" s="34"/>
+      <c r="F127" s="20"/>
+      <c r="G127" s="20"/>
+      <c r="H127" s="20"/>
+    </row>
+    <row r="128" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C128" s="34"/>
+      <c r="D128" s="34"/>
+      <c r="E128" s="34"/>
+      <c r="F128" s="20"/>
+      <c r="G128" s="20"/>
+      <c r="H128" s="20"/>
+    </row>
+    <row r="129" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C129" s="34"/>
+      <c r="D129" s="34"/>
+      <c r="E129" s="34"/>
+      <c r="F129" s="20"/>
+      <c r="G129" s="20"/>
+      <c r="H129" s="20"/>
+    </row>
+    <row r="130" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C130" s="34"/>
+      <c r="D130" s="34"/>
+      <c r="E130" s="34"/>
+      <c r="F130" s="20"/>
+      <c r="G130" s="20"/>
+      <c r="H130" s="20"/>
+    </row>
+    <row r="131" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C131" s="34"/>
+      <c r="D131" s="34"/>
+      <c r="E131" s="34"/>
+      <c r="F131" s="20"/>
+      <c r="G131" s="20"/>
+      <c r="H131" s="20"/>
+    </row>
+    <row r="132" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C132" s="34"/>
+      <c r="D132" s="34"/>
+      <c r="E132" s="34"/>
+      <c r="F132" s="20"/>
+      <c r="G132" s="20"/>
+      <c r="H132" s="20"/>
+    </row>
+    <row r="133" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C133" s="34"/>
+      <c r="D133" s="34"/>
+      <c r="E133" s="34"/>
+      <c r="F133" s="20"/>
+      <c r="G133" s="20"/>
+      <c r="H133" s="20"/>
+    </row>
+    <row r="134" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C134" s="34"/>
+      <c r="D134" s="34"/>
+      <c r="E134" s="34"/>
+      <c r="F134" s="20"/>
+      <c r="G134" s="20"/>
+      <c r="H134" s="20"/>
+    </row>
+    <row r="135" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C135" s="34"/>
+      <c r="D135" s="34"/>
+      <c r="E135" s="34"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="20"/>
+      <c r="H135" s="20"/>
+    </row>
+    <row r="136" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C136" s="34"/>
+      <c r="D136" s="34"/>
+      <c r="E136" s="34"/>
+      <c r="F136" s="20"/>
+      <c r="G136" s="20"/>
+      <c r="H136" s="20"/>
+    </row>
+    <row r="137" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C137" s="34"/>
+      <c r="D137" s="34"/>
+      <c r="E137" s="34"/>
+      <c r="F137" s="20"/>
+      <c r="G137" s="20"/>
+      <c r="H137" s="20"/>
+    </row>
+    <row r="138" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C138" s="34"/>
+      <c r="D138" s="34"/>
+      <c r="E138" s="34"/>
+      <c r="F138" s="20"/>
+      <c r="G138" s="20"/>
+      <c r="H138" s="20"/>
+    </row>
+    <row r="139" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C139" s="34"/>
+      <c r="D139" s="34"/>
+      <c r="E139" s="34"/>
+      <c r="F139" s="20"/>
+      <c r="G139" s="20"/>
+      <c r="H139" s="20"/>
+    </row>
+    <row r="140" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C140" s="34"/>
+      <c r="D140" s="34"/>
+      <c r="E140" s="34"/>
+      <c r="F140" s="20"/>
+      <c r="G140" s="20"/>
+      <c r="H140" s="20"/>
+    </row>
+    <row r="141" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C141" s="34"/>
+      <c r="D141" s="34"/>
+      <c r="E141" s="34"/>
+      <c r="F141" s="20"/>
+      <c r="G141" s="20"/>
+      <c r="H141" s="20"/>
+    </row>
+    <row r="142" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C142" s="34"/>
+      <c r="D142" s="34"/>
+      <c r="E142" s="34"/>
+      <c r="F142" s="20"/>
+      <c r="G142" s="20"/>
+      <c r="H142" s="20"/>
+    </row>
+    <row r="143" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C143" s="34"/>
+      <c r="D143" s="34"/>
+      <c r="E143" s="34"/>
+      <c r="F143" s="20"/>
+      <c r="G143" s="20"/>
+      <c r="H143" s="20"/>
+    </row>
+    <row r="144" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C144" s="34"/>
+      <c r="D144" s="34"/>
+      <c r="E144" s="34"/>
+      <c r="F144" s="20"/>
+      <c r="G144" s="20"/>
+      <c r="H144" s="20"/>
+    </row>
+    <row r="145" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C145" s="34"/>
+      <c r="D145" s="34"/>
+      <c r="E145" s="34"/>
+      <c r="F145" s="20"/>
+      <c r="G145" s="20"/>
+      <c r="H145" s="20"/>
+    </row>
+    <row r="146" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C146" s="34"/>
+      <c r="D146" s="34"/>
+      <c r="E146" s="34"/>
+      <c r="F146" s="20"/>
+      <c r="G146" s="20"/>
+      <c r="H146" s="20"/>
+    </row>
+    <row r="147" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C147" s="34"/>
+      <c r="D147" s="34"/>
+      <c r="E147" s="34"/>
+      <c r="F147" s="20"/>
+      <c r="G147" s="20"/>
+      <c r="H147" s="20"/>
+    </row>
+    <row r="148" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C148" s="34"/>
+      <c r="D148" s="34"/>
+      <c r="E148" s="34"/>
+      <c r="F148" s="20"/>
+      <c r="G148" s="20"/>
+      <c r="H148" s="20"/>
+    </row>
+    <row r="149" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C149" s="34"/>
+      <c r="D149" s="34"/>
+      <c r="E149" s="34"/>
+      <c r="F149" s="20"/>
+      <c r="G149" s="20"/>
+      <c r="H149" s="20"/>
+    </row>
+    <row r="150" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C150" s="34"/>
+      <c r="D150" s="34"/>
+      <c r="E150" s="34"/>
+      <c r="F150" s="20"/>
+      <c r="G150" s="20"/>
+      <c r="H150" s="20"/>
+    </row>
+    <row r="151" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C151" s="34"/>
+      <c r="D151" s="34"/>
+      <c r="E151" s="34"/>
+      <c r="F151" s="20"/>
+      <c r="G151" s="20"/>
+      <c r="H151" s="20"/>
+    </row>
+    <row r="152" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C152" s="34"/>
+      <c r="D152" s="34"/>
+      <c r="E152" s="34"/>
+      <c r="F152" s="20"/>
+      <c r="G152" s="20"/>
+      <c r="H152" s="20"/>
+    </row>
+    <row r="153" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C153" s="34"/>
+      <c r="D153" s="34"/>
+      <c r="E153" s="34"/>
+      <c r="F153" s="20"/>
+      <c r="G153" s="20"/>
+      <c r="H153" s="20"/>
+    </row>
+    <row r="154" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C154" s="34"/>
+      <c r="D154" s="34"/>
+      <c r="E154" s="34"/>
+      <c r="F154" s="20"/>
+      <c r="G154" s="20"/>
+      <c r="H154" s="20"/>
+    </row>
+    <row r="155" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C155" s="34"/>
+      <c r="D155" s="34"/>
+      <c r="E155" s="34"/>
+      <c r="F155" s="20"/>
+      <c r="G155" s="20"/>
+      <c r="H155" s="20"/>
+    </row>
+    <row r="156" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C156" s="34"/>
+      <c r="D156" s="34"/>
+      <c r="E156" s="34"/>
+      <c r="F156" s="20"/>
+      <c r="G156" s="20"/>
+      <c r="H156" s="20"/>
+    </row>
+    <row r="157" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C157" s="34"/>
+      <c r="D157" s="34"/>
+      <c r="E157" s="34"/>
+      <c r="F157" s="20"/>
+      <c r="G157" s="20"/>
+      <c r="H157" s="20"/>
+    </row>
+    <row r="158" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C158" s="34"/>
+      <c r="D158" s="34"/>
+      <c r="E158" s="34"/>
+      <c r="F158" s="20"/>
+      <c r="G158" s="20"/>
+      <c r="H158" s="20"/>
+    </row>
+    <row r="159" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C159" s="34"/>
+      <c r="D159" s="34"/>
+      <c r="E159" s="34"/>
+      <c r="F159" s="20"/>
+      <c r="G159" s="20"/>
+      <c r="H159" s="20"/>
+    </row>
+    <row r="160" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C160" s="34"/>
+      <c r="D160" s="34"/>
+      <c r="E160" s="34"/>
+      <c r="F160" s="20"/>
+      <c r="G160" s="20"/>
+      <c r="H160" s="20"/>
+    </row>
+    <row r="161" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C161" s="34"/>
+      <c r="D161" s="34"/>
+      <c r="E161" s="34"/>
+      <c r="F161" s="20"/>
+      <c r="G161" s="20"/>
+      <c r="H161" s="20"/>
+    </row>
+    <row r="162" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C162" s="34"/>
+      <c r="D162" s="34"/>
+      <c r="E162" s="34"/>
+      <c r="F162" s="20"/>
+      <c r="G162" s="20"/>
+      <c r="H162" s="20"/>
+    </row>
+    <row r="163" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C163" s="34"/>
+      <c r="D163" s="34"/>
+      <c r="E163" s="34"/>
+      <c r="F163" s="20"/>
+      <c r="G163" s="20"/>
+      <c r="H163" s="20"/>
+    </row>
+    <row r="164" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C164" s="34"/>
+      <c r="D164" s="34"/>
+      <c r="E164" s="34"/>
+      <c r="F164" s="20"/>
+      <c r="G164" s="20"/>
+      <c r="H164" s="20"/>
+    </row>
+    <row r="165" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C165" s="34"/>
+      <c r="D165" s="34"/>
+      <c r="E165" s="34"/>
+      <c r="F165" s="20"/>
+      <c r="G165" s="20"/>
+      <c r="H165" s="20"/>
+    </row>
+    <row r="166" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C166" s="34"/>
+      <c r="D166" s="34"/>
+      <c r="E166" s="34"/>
+      <c r="F166" s="20"/>
+      <c r="G166" s="20"/>
+      <c r="H166" s="20"/>
+    </row>
+    <row r="167" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C167" s="34"/>
+      <c r="D167" s="34"/>
+      <c r="E167" s="34"/>
+      <c r="F167" s="20"/>
+      <c r="G167" s="20"/>
+      <c r="H167" s="20"/>
+    </row>
+    <row r="168" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C168" s="34"/>
+      <c r="D168" s="34"/>
+      <c r="E168" s="34"/>
+      <c r="F168" s="20"/>
+      <c r="G168" s="20"/>
+      <c r="H168" s="20"/>
+    </row>
+    <row r="169" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C169" s="34"/>
+      <c r="D169" s="34"/>
+      <c r="E169" s="34"/>
+      <c r="F169" s="20"/>
+      <c r="G169" s="20"/>
+      <c r="H169" s="20"/>
+    </row>
+    <row r="170" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C170" s="34"/>
+      <c r="D170" s="34"/>
+      <c r="E170" s="34"/>
+      <c r="F170" s="20"/>
+      <c r="G170" s="20"/>
+      <c r="H170" s="20"/>
+    </row>
+    <row r="171" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C171" s="34"/>
+      <c r="D171" s="34"/>
+      <c r="E171" s="34"/>
+      <c r="F171" s="20"/>
+      <c r="G171" s="20"/>
+      <c r="H171" s="20"/>
+    </row>
+    <row r="172" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C172" s="34"/>
+      <c r="D172" s="34"/>
+      <c r="E172" s="34"/>
+      <c r="F172" s="20"/>
+      <c r="G172" s="20"/>
+      <c r="H172" s="20"/>
+    </row>
+    <row r="173" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C173" s="34"/>
+      <c r="D173" s="34"/>
+      <c r="E173" s="34"/>
+      <c r="F173" s="20"/>
+      <c r="G173" s="20"/>
+      <c r="H173" s="20"/>
+    </row>
+    <row r="174" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C174" s="34"/>
+      <c r="D174" s="34"/>
+      <c r="E174" s="34"/>
+      <c r="F174" s="20"/>
+      <c r="G174" s="20"/>
+      <c r="H174" s="20"/>
+    </row>
+    <row r="175" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C175" s="34"/>
+      <c r="D175" s="34"/>
+      <c r="E175" s="34"/>
+      <c r="F175" s="20"/>
+      <c r="G175" s="20"/>
+      <c r="H175" s="20"/>
+    </row>
+    <row r="176" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C176" s="34"/>
+      <c r="D176" s="34"/>
+      <c r="E176" s="34"/>
+      <c r="F176" s="20"/>
+      <c r="G176" s="20"/>
+      <c r="H176" s="20"/>
+    </row>
+    <row r="177" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C177" s="34"/>
+      <c r="D177" s="34"/>
+      <c r="E177" s="34"/>
+      <c r="F177" s="20"/>
+      <c r="G177" s="20"/>
+      <c r="H177" s="20"/>
+    </row>
+    <row r="178" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C178" s="34"/>
+      <c r="D178" s="34"/>
+      <c r="E178" s="34"/>
+      <c r="F178" s="20"/>
+      <c r="G178" s="20"/>
+      <c r="H178" s="20"/>
+    </row>
+    <row r="179" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C179" s="34"/>
+      <c r="D179" s="34"/>
+      <c r="E179" s="34"/>
+      <c r="F179" s="20"/>
+      <c r="G179" s="20"/>
+      <c r="H179" s="20"/>
+    </row>
+    <row r="180" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C180" s="34"/>
+      <c r="D180" s="34"/>
+      <c r="E180" s="34"/>
+      <c r="F180" s="20"/>
+      <c r="G180" s="20"/>
+      <c r="H180" s="20"/>
+    </row>
+    <row r="181" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C181" s="34"/>
+      <c r="D181" s="34"/>
+      <c r="E181" s="34"/>
+      <c r="F181" s="20"/>
+      <c r="G181" s="20"/>
+      <c r="H181" s="20"/>
+    </row>
+    <row r="182" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C182" s="34"/>
+      <c r="D182" s="34"/>
+      <c r="E182" s="34"/>
+      <c r="F182" s="20"/>
+      <c r="G182" s="20"/>
+      <c r="H182" s="20"/>
+    </row>
+    <row r="183" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C183" s="34"/>
+      <c r="D183" s="34"/>
+      <c r="E183" s="34"/>
+      <c r="F183" s="20"/>
+      <c r="G183" s="20"/>
+      <c r="H183" s="20"/>
+    </row>
+    <row r="184" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C184" s="34"/>
+      <c r="D184" s="34"/>
+      <c r="E184" s="34"/>
+      <c r="F184" s="20"/>
+      <c r="G184" s="20"/>
+      <c r="H184" s="20"/>
+    </row>
+    <row r="185" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C185" s="34"/>
+      <c r="D185" s="34"/>
+      <c r="E185" s="34"/>
+      <c r="F185" s="20"/>
+      <c r="G185" s="20"/>
+      <c r="H185" s="20"/>
+    </row>
+    <row r="186" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C186" s="34"/>
+      <c r="D186" s="34"/>
+      <c r="E186" s="34"/>
+      <c r="F186" s="20"/>
+      <c r="G186" s="20"/>
+      <c r="H186" s="20"/>
+    </row>
+    <row r="187" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C187" s="34"/>
+      <c r="D187" s="34"/>
+      <c r="E187" s="34"/>
+      <c r="F187" s="20"/>
+      <c r="G187" s="20"/>
+      <c r="H187" s="20"/>
+    </row>
+    <row r="188" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C188" s="34"/>
+      <c r="D188" s="34"/>
+      <c r="E188" s="34"/>
+      <c r="F188" s="20"/>
+      <c r="G188" s="20"/>
+      <c r="H188" s="20"/>
+    </row>
+    <row r="189" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C189" s="34"/>
+      <c r="D189" s="34"/>
+      <c r="E189" s="34"/>
+      <c r="F189" s="20"/>
+      <c r="G189" s="20"/>
+      <c r="H189" s="20"/>
+    </row>
+    <row r="190" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C190" s="34"/>
+      <c r="D190" s="34"/>
+      <c r="E190" s="34"/>
+      <c r="F190" s="20"/>
+      <c r="G190" s="20"/>
+      <c r="H190" s="20"/>
+    </row>
+    <row r="191" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C191" s="34"/>
+      <c r="D191" s="34"/>
+      <c r="E191" s="34"/>
+      <c r="F191" s="20"/>
+      <c r="G191" s="20"/>
+      <c r="H191" s="20"/>
+    </row>
+    <row r="192" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C192" s="34"/>
+      <c r="D192" s="34"/>
+      <c r="E192" s="34"/>
+      <c r="F192" s="20"/>
+      <c r="G192" s="20"/>
+      <c r="H192" s="20"/>
+    </row>
+    <row r="193" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C193" s="34"/>
+      <c r="D193" s="34"/>
+      <c r="E193" s="34"/>
+      <c r="F193" s="20"/>
+      <c r="G193" s="20"/>
+      <c r="H193" s="20"/>
+    </row>
+    <row r="194" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C194" s="34"/>
+      <c r="D194" s="34"/>
+      <c r="E194" s="34"/>
+      <c r="F194" s="20"/>
+      <c r="G194" s="20"/>
+      <c r="H194" s="20"/>
+    </row>
+    <row r="195" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C195" s="34"/>
+      <c r="D195" s="34"/>
+      <c r="E195" s="34"/>
+      <c r="F195" s="20"/>
+      <c r="G195" s="20"/>
+      <c r="H195" s="20"/>
+    </row>
+    <row r="196" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C196" s="34"/>
+      <c r="D196" s="34"/>
+      <c r="E196" s="34"/>
+      <c r="F196" s="20"/>
+      <c r="G196" s="20"/>
+      <c r="H196" s="20"/>
+    </row>
+    <row r="197" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C197" s="34"/>
+      <c r="D197" s="34"/>
+      <c r="E197" s="34"/>
+      <c r="F197" s="20"/>
+      <c r="G197" s="20"/>
+      <c r="H197" s="20"/>
+    </row>
+    <row r="198" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C198" s="34"/>
+      <c r="D198" s="34"/>
+      <c r="E198" s="34"/>
+      <c r="F198" s="20"/>
+      <c r="G198" s="20"/>
+      <c r="H198" s="20"/>
+    </row>
+    <row r="199" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C199" s="34"/>
+      <c r="D199" s="34"/>
+      <c r="E199" s="34"/>
+      <c r="F199" s="20"/>
+      <c r="G199" s="20"/>
+      <c r="H199" s="20"/>
+    </row>
+    <row r="200" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C200" s="34"/>
+      <c r="D200" s="34"/>
+      <c r="E200" s="34"/>
+      <c r="F200" s="20"/>
+      <c r="G200" s="20"/>
+      <c r="H200" s="20"/>
+    </row>
+    <row r="201" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C201" s="34"/>
+      <c r="D201" s="34"/>
+      <c r="E201" s="34"/>
+      <c r="F201" s="20"/>
+      <c r="G201" s="20"/>
+      <c r="H201" s="20"/>
+    </row>
+    <row r="202" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C202" s="34"/>
+      <c r="D202" s="34"/>
+      <c r="E202" s="34"/>
+      <c r="F202" s="20"/>
+      <c r="G202" s="20"/>
+      <c r="H202" s="20"/>
+    </row>
+    <row r="203" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C203" s="34"/>
+      <c r="D203" s="34"/>
+      <c r="E203" s="34"/>
+      <c r="F203" s="20"/>
+      <c r="G203" s="20"/>
+      <c r="H203" s="20"/>
+    </row>
+    <row r="204" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C204" s="34"/>
+      <c r="D204" s="34"/>
+      <c r="E204" s="34"/>
+      <c r="F204" s="20"/>
+      <c r="G204" s="20"/>
+      <c r="H204" s="20"/>
+    </row>
+    <row r="205" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C205" s="34"/>
+      <c r="D205" s="34"/>
+      <c r="E205" s="34"/>
+      <c r="F205" s="20"/>
+      <c r="G205" s="20"/>
+      <c r="H205" s="20"/>
+    </row>
+    <row r="206" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C206" s="34"/>
+      <c r="D206" s="34"/>
+      <c r="E206" s="34"/>
+      <c r="F206" s="20"/>
+      <c r="G206" s="20"/>
+      <c r="H206" s="20"/>
+    </row>
+    <row r="207" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C207" s="34"/>
+      <c r="D207" s="34"/>
+      <c r="E207" s="34"/>
+      <c r="F207" s="20"/>
+      <c r="G207" s="20"/>
+      <c r="H207" s="20"/>
+    </row>
+    <row r="208" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C208" s="34"/>
+      <c r="D208" s="34"/>
+      <c r="E208" s="34"/>
+      <c r="F208" s="20"/>
+      <c r="G208" s="20"/>
+      <c r="H208" s="20"/>
+    </row>
+    <row r="209" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C209" s="34"/>
+      <c r="D209" s="34"/>
+      <c r="E209" s="34"/>
+      <c r="F209" s="20"/>
+      <c r="G209" s="20"/>
+      <c r="H209" s="20"/>
+    </row>
+    <row r="210" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C210" s="34"/>
+      <c r="D210" s="34"/>
+      <c r="E210" s="34"/>
+      <c r="F210" s="20"/>
+      <c r="G210" s="20"/>
+      <c r="H210" s="20"/>
+    </row>
+    <row r="211" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C211" s="34"/>
+      <c r="D211" s="34"/>
+      <c r="E211" s="34"/>
+      <c r="F211" s="20"/>
+      <c r="G211" s="20"/>
+      <c r="H211" s="20"/>
+    </row>
+    <row r="212" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C212" s="34"/>
+      <c r="D212" s="34"/>
+      <c r="E212" s="34"/>
+      <c r="F212" s="20"/>
+      <c r="G212" s="20"/>
+      <c r="H212" s="20"/>
+    </row>
+    <row r="213" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C213" s="34"/>
+      <c r="D213" s="34"/>
+      <c r="E213" s="34"/>
+      <c r="F213" s="20"/>
+      <c r="G213" s="20"/>
+      <c r="H213" s="20"/>
+    </row>
+    <row r="214" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C214" s="34"/>
+      <c r="D214" s="34"/>
+      <c r="E214" s="34"/>
+      <c r="F214" s="20"/>
+      <c r="G214" s="20"/>
+      <c r="H214" s="20"/>
+    </row>
+    <row r="215" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C215" s="34"/>
+      <c r="D215" s="34"/>
+      <c r="E215" s="34"/>
+      <c r="F215" s="20"/>
+      <c r="G215" s="20"/>
+      <c r="H215" s="20"/>
+    </row>
+    <row r="216" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C216" s="34"/>
+      <c r="D216" s="34"/>
+      <c r="E216" s="34"/>
+      <c r="F216" s="20"/>
+      <c r="G216" s="20"/>
+      <c r="H216" s="20"/>
+    </row>
+    <row r="217" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C217" s="34"/>
+      <c r="D217" s="34"/>
+      <c r="E217" s="34"/>
+      <c r="F217" s="20"/>
+      <c r="G217" s="20"/>
+      <c r="H217" s="20"/>
+    </row>
+    <row r="218" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C218" s="34"/>
+      <c r="D218" s="34"/>
+      <c r="E218" s="34"/>
+      <c r="F218" s="20"/>
+      <c r="G218" s="20"/>
+      <c r="H218" s="20"/>
+    </row>
+    <row r="219" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C219" s="34"/>
+      <c r="D219" s="34"/>
+      <c r="E219" s="34"/>
+      <c r="F219" s="20"/>
+      <c r="G219" s="20"/>
+      <c r="H219" s="20"/>
+    </row>
+    <row r="220" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C220" s="34"/>
+      <c r="D220" s="34"/>
+      <c r="E220" s="34"/>
+      <c r="F220" s="20"/>
+      <c r="G220" s="20"/>
+      <c r="H220" s="20"/>
+    </row>
+    <row r="221" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C221" s="34"/>
+      <c r="D221" s="34"/>
+      <c r="E221" s="34"/>
+      <c r="F221" s="20"/>
+      <c r="G221" s="20"/>
+      <c r="H221" s="20"/>
+    </row>
+    <row r="222" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C222" s="34"/>
+      <c r="D222" s="34"/>
+      <c r="E222" s="34"/>
+      <c r="F222" s="20"/>
+      <c r="G222" s="20"/>
+      <c r="H222" s="20"/>
+    </row>
+    <row r="223" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C223" s="34"/>
+      <c r="D223" s="34"/>
+      <c r="E223" s="34"/>
+      <c r="F223" s="20"/>
+      <c r="G223" s="20"/>
+      <c r="H223" s="20"/>
+    </row>
+    <row r="224" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C224" s="34"/>
+      <c r="D224" s="34"/>
+      <c r="E224" s="34"/>
+      <c r="F224" s="20"/>
+      <c r="G224" s="20"/>
+      <c r="H224" s="20"/>
+    </row>
+    <row r="225" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C225" s="34"/>
+      <c r="D225" s="34"/>
+      <c r="E225" s="34"/>
+      <c r="F225" s="20"/>
+      <c r="G225" s="20"/>
+      <c r="H225" s="20"/>
+    </row>
+    <row r="226" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C226" s="34"/>
+      <c r="D226" s="34"/>
+      <c r="E226" s="34"/>
+      <c r="F226" s="20"/>
+      <c r="G226" s="20"/>
+      <c r="H226" s="20"/>
+    </row>
+    <row r="227" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C227" s="34"/>
+      <c r="D227" s="34"/>
+      <c r="E227" s="34"/>
+      <c r="F227" s="20"/>
+      <c r="G227" s="20"/>
+      <c r="H227" s="20"/>
+    </row>
+    <row r="228" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C228" s="34"/>
+      <c r="D228" s="34"/>
+      <c r="E228" s="34"/>
+      <c r="F228" s="20"/>
+      <c r="G228" s="20"/>
+      <c r="H228" s="20"/>
+    </row>
+    <row r="229" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C229" s="34"/>
+      <c r="D229" s="34"/>
+      <c r="E229" s="34"/>
+      <c r="F229" s="20"/>
+      <c r="G229" s="20"/>
+      <c r="H229" s="20"/>
+    </row>
+    <row r="230" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C230" s="34"/>
+      <c r="D230" s="34"/>
+      <c r="E230" s="34"/>
+      <c r="F230" s="20"/>
+      <c r="G230" s="20"/>
+      <c r="H230" s="20"/>
+    </row>
+    <row r="231" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C231" s="34"/>
+      <c r="D231" s="34"/>
+      <c r="E231" s="34"/>
+      <c r="F231" s="20"/>
+      <c r="G231" s="20"/>
+      <c r="H231" s="20"/>
+    </row>
+    <row r="232" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C232" s="34"/>
+      <c r="D232" s="34"/>
+      <c r="E232" s="34"/>
+      <c r="F232" s="20"/>
+      <c r="G232" s="20"/>
+      <c r="H232" s="20"/>
+    </row>
+    <row r="233" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C233" s="34"/>
+      <c r="D233" s="34"/>
+      <c r="E233" s="34"/>
+      <c r="F233" s="20"/>
+      <c r="G233" s="20"/>
+      <c r="H233" s="20"/>
+    </row>
+    <row r="234" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C234" s="34"/>
+      <c r="D234" s="34"/>
+      <c r="E234" s="34"/>
+      <c r="F234" s="20"/>
+      <c r="G234" s="20"/>
+      <c r="H234" s="20"/>
+    </row>
+    <row r="235" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C235" s="34"/>
+      <c r="D235" s="34"/>
+      <c r="E235" s="34"/>
+      <c r="F235" s="20"/>
+      <c r="G235" s="20"/>
+      <c r="H235" s="20"/>
+    </row>
+    <row r="236" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C236" s="34"/>
+      <c r="D236" s="34"/>
+      <c r="E236" s="34"/>
+      <c r="F236" s="20"/>
+      <c r="G236" s="20"/>
+      <c r="H236" s="20"/>
+    </row>
+    <row r="237" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C237" s="34"/>
+      <c r="D237" s="34"/>
+      <c r="E237" s="34"/>
+      <c r="F237" s="20"/>
+      <c r="G237" s="20"/>
+      <c r="H237" s="20"/>
+    </row>
+    <row r="238" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C238" s="34"/>
+      <c r="D238" s="34"/>
+      <c r="E238" s="34"/>
+      <c r="F238" s="20"/>
+      <c r="G238" s="20"/>
+      <c r="H238" s="20"/>
+    </row>
+    <row r="239" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C239" s="34"/>
+      <c r="D239" s="34"/>
+      <c r="E239" s="34"/>
+      <c r="F239" s="20"/>
+      <c r="G239" s="20"/>
+      <c r="H239" s="20"/>
+    </row>
+    <row r="240" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C240" s="34"/>
+      <c r="D240" s="34"/>
+      <c r="E240" s="34"/>
+      <c r="F240" s="20"/>
+      <c r="G240" s="20"/>
+      <c r="H240" s="20"/>
+    </row>
+    <row r="241" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C241" s="34"/>
+      <c r="D241" s="34"/>
+      <c r="E241" s="34"/>
+      <c r="F241" s="20"/>
+      <c r="G241" s="20"/>
+      <c r="H241" s="20"/>
+    </row>
+    <row r="242" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C242" s="34"/>
+      <c r="D242" s="34"/>
+      <c r="E242" s="34"/>
+      <c r="F242" s="20"/>
+      <c r="G242" s="20"/>
+      <c r="H242" s="20"/>
+    </row>
+    <row r="243" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C243" s="34"/>
+      <c r="D243" s="34"/>
+      <c r="E243" s="34"/>
+      <c r="F243" s="20"/>
+      <c r="G243" s="20"/>
+      <c r="H243" s="20"/>
+    </row>
+    <row r="244" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C244" s="34"/>
+      <c r="D244" s="34"/>
+      <c r="E244" s="34"/>
+      <c r="F244" s="20"/>
+      <c r="G244" s="20"/>
+      <c r="H244" s="20"/>
+    </row>
+    <row r="245" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C245" s="34"/>
+      <c r="D245" s="34"/>
+      <c r="E245" s="34"/>
+      <c r="F245" s="20"/>
+      <c r="G245" s="20"/>
+      <c r="H245" s="20"/>
+    </row>
+    <row r="246" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C246" s="34"/>
+      <c r="D246" s="34"/>
+      <c r="E246" s="34"/>
+      <c r="F246" s="20"/>
+      <c r="G246" s="20"/>
+      <c r="H246" s="20"/>
+    </row>
+    <row r="247" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C247" s="34"/>
+      <c r="D247" s="34"/>
+      <c r="E247" s="34"/>
+      <c r="F247" s="20"/>
+      <c r="G247" s="20"/>
+      <c r="H247" s="20"/>
+    </row>
+    <row r="248" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C248" s="34"/>
+      <c r="D248" s="34"/>
+      <c r="E248" s="34"/>
+      <c r="F248" s="20"/>
+      <c r="G248" s="20"/>
+      <c r="H248" s="20"/>
+    </row>
+    <row r="249" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C249" s="34"/>
+      <c r="D249" s="34"/>
+      <c r="E249" s="34"/>
+      <c r="F249" s="20"/>
+      <c r="G249" s="20"/>
+      <c r="H249" s="20"/>
+    </row>
+    <row r="250" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C250" s="34"/>
+      <c r="D250" s="34"/>
+      <c r="E250" s="34"/>
+      <c r="F250" s="20"/>
+      <c r="G250" s="20"/>
+      <c r="H250" s="20"/>
+    </row>
+    <row r="251" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C251" s="34"/>
+      <c r="D251" s="34"/>
+      <c r="E251" s="34"/>
+      <c r="F251" s="20"/>
+      <c r="G251" s="20"/>
+      <c r="H251" s="20"/>
+    </row>
+    <row r="252" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C252" s="34"/>
+      <c r="D252" s="34"/>
+      <c r="E252" s="34"/>
+      <c r="F252" s="20"/>
+      <c r="G252" s="20"/>
+      <c r="H252" s="20"/>
+    </row>
+    <row r="253" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C253" s="34"/>
+      <c r="D253" s="34"/>
+      <c r="E253" s="34"/>
+      <c r="F253" s="20"/>
+      <c r="G253" s="20"/>
+      <c r="H253" s="20"/>
+    </row>
+    <row r="254" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C254" s="34"/>
+      <c r="D254" s="34"/>
+      <c r="E254" s="34"/>
+      <c r="F254" s="20"/>
+      <c r="G254" s="20"/>
+      <c r="H254" s="20"/>
+    </row>
+    <row r="255" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C255" s="34"/>
+      <c r="D255" s="34"/>
+      <c r="E255" s="34"/>
+      <c r="F255" s="20"/>
+      <c r="G255" s="20"/>
+      <c r="H255" s="20"/>
+    </row>
+    <row r="256" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C256" s="34"/>
+      <c r="D256" s="34"/>
+      <c r="E256" s="34"/>
+      <c r="F256" s="20"/>
+      <c r="G256" s="20"/>
+      <c r="H256" s="20"/>
+    </row>
+    <row r="257" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C257" s="34"/>
+      <c r="D257" s="34"/>
+      <c r="E257" s="34"/>
+      <c r="F257" s="20"/>
+      <c r="G257" s="20"/>
+      <c r="H257" s="20"/>
+    </row>
+    <row r="258" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C258" s="34"/>
+      <c r="D258" s="34"/>
+      <c r="E258" s="34"/>
+      <c r="F258" s="20"/>
+      <c r="G258" s="20"/>
+      <c r="H258" s="20"/>
+    </row>
+    <row r="259" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C259" s="34"/>
+      <c r="D259" s="34"/>
+      <c r="E259" s="34"/>
+      <c r="F259" s="20"/>
+      <c r="G259" s="20"/>
+      <c r="H259" s="20"/>
+    </row>
+    <row r="260" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C260" s="34"/>
+      <c r="D260" s="34"/>
+      <c r="E260" s="34"/>
+      <c r="F260" s="20"/>
+      <c r="G260" s="20"/>
+      <c r="H260" s="20"/>
+    </row>
+    <row r="261" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C261" s="34"/>
+      <c r="D261" s="34"/>
+      <c r="E261" s="34"/>
+      <c r="F261" s="20"/>
+      <c r="G261" s="20"/>
+      <c r="H261" s="20"/>
+    </row>
+    <row r="262" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C262" s="34"/>
+      <c r="D262" s="34"/>
+      <c r="E262" s="34"/>
+      <c r="F262" s="20"/>
+      <c r="G262" s="20"/>
+      <c r="H262" s="20"/>
+    </row>
+    <row r="263" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C263" s="34"/>
+      <c r="D263" s="34"/>
+      <c r="E263" s="34"/>
+      <c r="F263" s="20"/>
+      <c r="G263" s="20"/>
+      <c r="H263" s="20"/>
+    </row>
+    <row r="264" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C264" s="34"/>
+      <c r="D264" s="34"/>
+      <c r="E264" s="34"/>
+      <c r="F264" s="20"/>
+      <c r="G264" s="20"/>
+      <c r="H264" s="20"/>
+    </row>
+    <row r="265" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C265" s="34"/>
+      <c r="D265" s="34"/>
+      <c r="E265" s="34"/>
+      <c r="F265" s="20"/>
+      <c r="G265" s="20"/>
+      <c r="H265" s="20"/>
+    </row>
+    <row r="266" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C266" s="34"/>
+      <c r="D266" s="34"/>
+      <c r="E266" s="34"/>
+      <c r="F266" s="20"/>
+      <c r="G266" s="20"/>
+      <c r="H266" s="20"/>
+    </row>
+    <row r="267" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C267" s="34"/>
+      <c r="D267" s="34"/>
+      <c r="E267" s="34"/>
+      <c r="F267" s="20"/>
+      <c r="G267" s="20"/>
+      <c r="H267" s="20"/>
+    </row>
+    <row r="268" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C268" s="34"/>
+      <c r="D268" s="34"/>
+      <c r="E268" s="34"/>
+      <c r="F268" s="20"/>
+      <c r="G268" s="20"/>
+      <c r="H268" s="20"/>
+    </row>
+    <row r="269" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C269" s="34"/>
+      <c r="D269" s="34"/>
+      <c r="E269" s="34"/>
+      <c r="F269" s="20"/>
+      <c r="G269" s="20"/>
+      <c r="H269" s="20"/>
+    </row>
+    <row r="270" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C270" s="34"/>
+      <c r="D270" s="34"/>
+      <c r="E270" s="34"/>
+      <c r="F270" s="20"/>
+      <c r="G270" s="20"/>
+      <c r="H270" s="20"/>
+    </row>
+    <row r="271" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C271" s="34"/>
+      <c r="D271" s="34"/>
+      <c r="E271" s="34"/>
+      <c r="F271" s="20"/>
+      <c r="G271" s="20"/>
+      <c r="H271" s="20"/>
+    </row>
+    <row r="272" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C272" s="34"/>
+      <c r="D272" s="34"/>
+      <c r="E272" s="34"/>
+      <c r="F272" s="20"/>
+      <c r="G272" s="20"/>
+      <c r="H272" s="20"/>
+    </row>
+    <row r="273" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C273" s="34"/>
+      <c r="D273" s="34"/>
+      <c r="E273" s="34"/>
+      <c r="F273" s="20"/>
+      <c r="G273" s="20"/>
+      <c r="H273" s="20"/>
+    </row>
+    <row r="274" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C274" s="34"/>
+      <c r="D274" s="34"/>
+      <c r="E274" s="34"/>
+      <c r="F274" s="20"/>
+      <c r="G274" s="20"/>
+      <c r="H274" s="20"/>
+    </row>
+    <row r="275" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C275" s="34"/>
+      <c r="D275" s="34"/>
+      <c r="E275" s="34"/>
+      <c r="F275" s="20"/>
+      <c r="G275" s="20"/>
+      <c r="H275" s="20"/>
+    </row>
+    <row r="276" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C276" s="34"/>
+      <c r="D276" s="34"/>
+      <c r="E276" s="34"/>
+      <c r="F276" s="20"/>
+      <c r="G276" s="20"/>
+      <c r="H276" s="20"/>
+    </row>
+    <row r="277" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C277" s="34"/>
+      <c r="D277" s="34"/>
+      <c r="E277" s="34"/>
+      <c r="F277" s="20"/>
+      <c r="G277" s="20"/>
+      <c r="H277" s="20"/>
+    </row>
+    <row r="278" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C278" s="34"/>
+      <c r="D278" s="34"/>
+      <c r="E278" s="34"/>
+      <c r="F278" s="20"/>
+      <c r="G278" s="20"/>
+      <c r="H278" s="20"/>
+    </row>
+    <row r="279" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C279" s="34"/>
+      <c r="D279" s="34"/>
+      <c r="E279" s="34"/>
+      <c r="F279" s="20"/>
+      <c r="G279" s="20"/>
+      <c r="H279" s="20"/>
+    </row>
+    <row r="280" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C280" s="34"/>
+      <c r="D280" s="34"/>
+      <c r="E280" s="34"/>
+      <c r="F280" s="20"/>
+      <c r="G280" s="20"/>
+      <c r="H280" s="20"/>
+    </row>
+    <row r="281" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C281" s="34"/>
+      <c r="D281" s="34"/>
+      <c r="E281" s="34"/>
+      <c r="F281" s="20"/>
+      <c r="G281" s="20"/>
+      <c r="H281" s="20"/>
+    </row>
+    <row r="282" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C282" s="34"/>
+      <c r="D282" s="34"/>
+      <c r="E282" s="34"/>
+      <c r="F282" s="20"/>
+      <c r="G282" s="20"/>
+      <c r="H282" s="20"/>
+    </row>
+    <row r="283" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C283" s="34"/>
+      <c r="D283" s="34"/>
+      <c r="E283" s="34"/>
+      <c r="F283" s="20"/>
+      <c r="G283" s="20"/>
+      <c r="H283" s="20"/>
+    </row>
+    <row r="284" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C284" s="34"/>
+      <c r="D284" s="34"/>
+      <c r="E284" s="34"/>
+      <c r="F284" s="20"/>
+      <c r="G284" s="20"/>
+      <c r="H284" s="20"/>
+    </row>
+    <row r="285" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C285" s="34"/>
+      <c r="D285" s="34"/>
+      <c r="E285" s="34"/>
+      <c r="F285" s="20"/>
+      <c r="G285" s="20"/>
+      <c r="H285" s="20"/>
+    </row>
+    <row r="286" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C286" s="34"/>
+      <c r="D286" s="34"/>
+      <c r="E286" s="34"/>
+      <c r="F286" s="20"/>
+      <c r="G286" s="20"/>
+      <c r="H286" s="20"/>
+    </row>
+    <row r="287" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C287" s="34"/>
+      <c r="D287" s="34"/>
+      <c r="E287" s="34"/>
+      <c r="F287" s="20"/>
+      <c r="G287" s="20"/>
+      <c r="H287" s="20"/>
+    </row>
+    <row r="288" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C288" s="34"/>
+      <c r="D288" s="34"/>
+      <c r="E288" s="34"/>
+      <c r="F288" s="20"/>
+      <c r="G288" s="20"/>
+      <c r="H288" s="20"/>
+    </row>
+    <row r="289" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C289" s="34"/>
+      <c r="D289" s="34"/>
+      <c r="E289" s="34"/>
+      <c r="F289" s="20"/>
+      <c r="G289" s="20"/>
+      <c r="H289" s="20"/>
+    </row>
+    <row r="290" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C290" s="34"/>
+      <c r="D290" s="34"/>
+      <c r="E290" s="34"/>
+      <c r="F290" s="20"/>
+      <c r="G290" s="20"/>
+      <c r="H290" s="20"/>
+    </row>
+    <row r="291" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C291" s="34"/>
+      <c r="D291" s="34"/>
+      <c r="E291" s="34"/>
+      <c r="F291" s="20"/>
+      <c r="G291" s="20"/>
+      <c r="H291" s="20"/>
+    </row>
+    <row r="292" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C292" s="34"/>
+      <c r="D292" s="34"/>
+      <c r="E292" s="34"/>
+      <c r="F292" s="20"/>
+      <c r="G292" s="20"/>
+      <c r="H292" s="20"/>
+    </row>
+    <row r="293" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C293" s="34"/>
+      <c r="D293" s="34"/>
+      <c r="E293" s="34"/>
+      <c r="F293" s="20"/>
+      <c r="G293" s="20"/>
+      <c r="H293" s="20"/>
+    </row>
+    <row r="294" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C294" s="34"/>
+      <c r="D294" s="34"/>
+      <c r="E294" s="34"/>
+      <c r="F294" s="20"/>
+      <c r="G294" s="20"/>
+      <c r="H294" s="20"/>
+    </row>
+    <row r="295" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C295" s="34"/>
+      <c r="D295" s="34"/>
+      <c r="E295" s="34"/>
+      <c r="F295" s="20"/>
+      <c r="G295" s="20"/>
+      <c r="H295" s="20"/>
+    </row>
+    <row r="296" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C296" s="34"/>
+      <c r="D296" s="34"/>
+      <c r="E296" s="34"/>
+      <c r="F296" s="20"/>
+      <c r="G296" s="20"/>
+      <c r="H296" s="20"/>
+    </row>
+    <row r="297" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C297" s="34"/>
+      <c r="D297" s="34"/>
+      <c r="E297" s="34"/>
+      <c r="F297" s="20"/>
+      <c r="G297" s="20"/>
+      <c r="H297" s="20"/>
+    </row>
+    <row r="298" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C298" s="34"/>
+      <c r="D298" s="34"/>
+      <c r="E298" s="34"/>
+      <c r="F298" s="20"/>
+      <c r="G298" s="20"/>
+      <c r="H298" s="20"/>
+    </row>
+    <row r="299" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C299" s="34"/>
+      <c r="D299" s="34"/>
+      <c r="E299" s="34"/>
+      <c r="F299" s="20"/>
+      <c r="G299" s="20"/>
+      <c r="H299" s="20"/>
+    </row>
+    <row r="300" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C300" s="34"/>
+      <c r="D300" s="34"/>
+      <c r="E300" s="34"/>
+      <c r="F300" s="20"/>
+      <c r="G300" s="20"/>
+      <c r="H300" s="20"/>
+    </row>
+    <row r="301" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C301" s="34"/>
+      <c r="D301" s="34"/>
+      <c r="E301" s="34"/>
+      <c r="F301" s="20"/>
+      <c r="G301" s="20"/>
+      <c r="H301" s="20"/>
+    </row>
+    <row r="302" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C302" s="34"/>
+      <c r="D302" s="34"/>
+      <c r="E302" s="34"/>
+      <c r="F302" s="20"/>
+      <c r="G302" s="20"/>
+      <c r="H302" s="20"/>
+    </row>
+    <row r="303" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C303" s="34"/>
+      <c r="D303" s="34"/>
+      <c r="E303" s="34"/>
+      <c r="F303" s="20"/>
+      <c r="G303" s="20"/>
+      <c r="H303" s="20"/>
+    </row>
+    <row r="304" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C304" s="34"/>
+      <c r="D304" s="34"/>
+      <c r="E304" s="34"/>
+      <c r="F304" s="20"/>
+      <c r="G304" s="20"/>
+      <c r="H304" s="20"/>
+    </row>
+    <row r="305" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C305" s="34"/>
+      <c r="D305" s="34"/>
+      <c r="E305" s="34"/>
+      <c r="F305" s="20"/>
+      <c r="G305" s="20"/>
+      <c r="H305" s="20"/>
+    </row>
+    <row r="306" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C306" s="34"/>
+      <c r="D306" s="34"/>
+      <c r="E306" s="34"/>
+      <c r="F306" s="20"/>
+      <c r="G306" s="20"/>
+      <c r="H306" s="20"/>
+    </row>
+    <row r="307" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C307" s="34"/>
+      <c r="D307" s="34"/>
+      <c r="E307" s="34"/>
+      <c r="F307" s="20"/>
+      <c r="G307" s="20"/>
+      <c r="H307" s="20"/>
+    </row>
+    <row r="308" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C308" s="34"/>
+      <c r="D308" s="34"/>
+      <c r="E308" s="34"/>
+      <c r="F308" s="20"/>
+      <c r="G308" s="20"/>
+      <c r="H308" s="20"/>
+    </row>
+    <row r="309" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C309" s="34"/>
+      <c r="D309" s="34"/>
+      <c r="E309" s="34"/>
+      <c r="F309" s="20"/>
+      <c r="G309" s="20"/>
+      <c r="H309" s="20"/>
+    </row>
+    <row r="310" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C310" s="34"/>
+      <c r="D310" s="34"/>
+      <c r="E310" s="34"/>
+      <c r="F310" s="20"/>
+      <c r="G310" s="20"/>
+      <c r="H310" s="20"/>
+    </row>
+    <row r="311" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C311" s="34"/>
+      <c r="D311" s="34"/>
+      <c r="E311" s="34"/>
+      <c r="F311" s="20"/>
+      <c r="G311" s="20"/>
+      <c r="H311" s="20"/>
+    </row>
+    <row r="312" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C312" s="34"/>
+      <c r="D312" s="34"/>
+      <c r="E312" s="34"/>
+      <c r="F312" s="20"/>
+      <c r="G312" s="20"/>
+      <c r="H312" s="20"/>
+    </row>
+    <row r="313" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C313" s="34"/>
+      <c r="D313" s="34"/>
+      <c r="E313" s="34"/>
+      <c r="F313" s="20"/>
+      <c r="G313" s="20"/>
+      <c r="H313" s="20"/>
+    </row>
+    <row r="314" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C314" s="34"/>
+      <c r="D314" s="34"/>
+      <c r="E314" s="34"/>
+      <c r="F314" s="20"/>
+      <c r="G314" s="20"/>
+      <c r="H314" s="20"/>
+    </row>
+    <row r="315" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C315" s="34"/>
+      <c r="D315" s="34"/>
+      <c r="E315" s="34"/>
+      <c r="F315" s="20"/>
+      <c r="G315" s="20"/>
+      <c r="H315" s="20"/>
+    </row>
+    <row r="316" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C316" s="34"/>
+      <c r="D316" s="34"/>
+      <c r="E316" s="34"/>
+      <c r="F316" s="20"/>
+      <c r="G316" s="20"/>
+      <c r="H316" s="20"/>
+    </row>
+    <row r="317" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C317" s="34"/>
+      <c r="D317" s="34"/>
+      <c r="E317" s="34"/>
+      <c r="F317" s="20"/>
+      <c r="G317" s="20"/>
+      <c r="H317" s="20"/>
+    </row>
+    <row r="318" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C318" s="34"/>
+      <c r="D318" s="34"/>
+      <c r="E318" s="34"/>
+      <c r="F318" s="20"/>
+      <c r="G318" s="20"/>
+      <c r="H318" s="20"/>
+    </row>
+    <row r="319" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C319" s="34"/>
+      <c r="D319" s="34"/>
+      <c r="E319" s="34"/>
+      <c r="F319" s="20"/>
+      <c r="G319" s="20"/>
+      <c r="H319" s="20"/>
+    </row>
+    <row r="320" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C320" s="34"/>
+      <c r="D320" s="34"/>
+      <c r="E320" s="34"/>
+      <c r="F320" s="20"/>
+      <c r="G320" s="20"/>
+      <c r="H320" s="20"/>
+    </row>
+    <row r="321" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C321" s="34"/>
+      <c r="D321" s="34"/>
+      <c r="E321" s="34"/>
+      <c r="F321" s="20"/>
+      <c r="G321" s="20"/>
+      <c r="H321" s="20"/>
+    </row>
+    <row r="322" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C322" s="34"/>
+      <c r="D322" s="34"/>
+      <c r="E322" s="34"/>
+      <c r="F322" s="20"/>
+      <c r="G322" s="20"/>
+      <c r="H322" s="20"/>
+    </row>
+    <row r="323" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C323" s="34"/>
+      <c r="D323" s="34"/>
+      <c r="E323" s="34"/>
+      <c r="F323" s="20"/>
+      <c r="G323" s="20"/>
+      <c r="H323" s="20"/>
+    </row>
+    <row r="324" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C324" s="34"/>
+      <c r="D324" s="34"/>
+      <c r="E324" s="34"/>
+      <c r="F324" s="20"/>
+      <c r="G324" s="20"/>
+      <c r="H324" s="20"/>
+    </row>
+    <row r="325" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C325" s="34"/>
+      <c r="D325" s="34"/>
+      <c r="E325" s="34"/>
+      <c r="F325" s="20"/>
+      <c r="G325" s="20"/>
+      <c r="H325" s="20"/>
+    </row>
+    <row r="326" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C326" s="34"/>
+      <c r="D326" s="34"/>
+      <c r="E326" s="34"/>
+      <c r="F326" s="20"/>
+      <c r="G326" s="20"/>
+      <c r="H326" s="20"/>
+    </row>
+    <row r="327" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C327" s="34"/>
+      <c r="D327" s="34"/>
+      <c r="E327" s="34"/>
+      <c r="F327" s="20"/>
+      <c r="G327" s="20"/>
+      <c r="H327" s="20"/>
+    </row>
+    <row r="328" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C328" s="34"/>
+      <c r="D328" s="34"/>
+      <c r="E328" s="34"/>
+      <c r="F328" s="20"/>
+      <c r="G328" s="20"/>
+      <c r="H328" s="20"/>
+    </row>
+    <row r="329" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C329" s="34"/>
+      <c r="D329" s="34"/>
+      <c r="E329" s="34"/>
+      <c r="F329" s="20"/>
+      <c r="G329" s="20"/>
+      <c r="H329" s="20"/>
+    </row>
+    <row r="330" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C330" s="34"/>
+      <c r="D330" s="34"/>
+      <c r="E330" s="34"/>
+      <c r="F330" s="20"/>
+      <c r="G330" s="20"/>
+      <c r="H330" s="20"/>
+    </row>
+    <row r="331" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C331" s="34"/>
+      <c r="D331" s="34"/>
+      <c r="E331" s="34"/>
+      <c r="F331" s="20"/>
+      <c r="G331" s="20"/>
+      <c r="H331" s="20"/>
+    </row>
+    <row r="332" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C332" s="34"/>
+      <c r="D332" s="34"/>
+      <c r="E332" s="34"/>
+      <c r="F332" s="20"/>
+      <c r="G332" s="20"/>
+      <c r="H332" s="20"/>
+    </row>
+    <row r="333" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C333" s="34"/>
+      <c r="D333" s="34"/>
+      <c r="E333" s="34"/>
+      <c r="F333" s="20"/>
+      <c r="G333" s="20"/>
+      <c r="H333" s="20"/>
+    </row>
+    <row r="334" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C334" s="34"/>
+      <c r="D334" s="34"/>
+      <c r="E334" s="34"/>
+      <c r="F334" s="20"/>
+      <c r="G334" s="20"/>
+      <c r="H334" s="20"/>
+    </row>
+    <row r="335" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C335" s="34"/>
+      <c r="D335" s="34"/>
+      <c r="E335" s="34"/>
+      <c r="F335" s="20"/>
+      <c r="G335" s="20"/>
+      <c r="H335" s="20"/>
+    </row>
+    <row r="336" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C336" s="34"/>
+      <c r="D336" s="34"/>
+      <c r="E336" s="34"/>
+      <c r="F336" s="20"/>
+      <c r="G336" s="20"/>
+      <c r="H336" s="20"/>
+    </row>
+    <row r="337" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C337" s="34"/>
+      <c r="D337" s="34"/>
+      <c r="E337" s="34"/>
+      <c r="F337" s="20"/>
+      <c r="G337" s="20"/>
+      <c r="H337" s="20"/>
+    </row>
+    <row r="338" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C338" s="34"/>
+      <c r="D338" s="34"/>
+      <c r="E338" s="34"/>
+      <c r="F338" s="20"/>
+      <c r="G338" s="20"/>
+      <c r="H338" s="20"/>
+    </row>
+    <row r="339" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C339" s="34"/>
+      <c r="D339" s="34"/>
+      <c r="E339" s="34"/>
+      <c r="F339" s="20"/>
+      <c r="G339" s="20"/>
+      <c r="H339" s="20"/>
+    </row>
+    <row r="340" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C340" s="34"/>
+      <c r="D340" s="34"/>
+      <c r="E340" s="34"/>
+      <c r="F340" s="20"/>
+      <c r="G340" s="20"/>
+      <c r="H340" s="20"/>
+    </row>
+    <row r="341" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C341" s="34"/>
+      <c r="D341" s="34"/>
+      <c r="E341" s="34"/>
+      <c r="F341" s="20"/>
+      <c r="G341" s="20"/>
+      <c r="H341" s="20"/>
+    </row>
+    <row r="342" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C342" s="34"/>
+      <c r="D342" s="34"/>
+      <c r="E342" s="34"/>
+      <c r="F342" s="20"/>
+      <c r="G342" s="20"/>
+      <c r="H342" s="20"/>
+    </row>
+    <row r="343" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C343" s="34"/>
+      <c r="D343" s="34"/>
+      <c r="E343" s="34"/>
+      <c r="F343" s="20"/>
+      <c r="G343" s="20"/>
+      <c r="H343" s="20"/>
+    </row>
+    <row r="344" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C344" s="34"/>
+      <c r="D344" s="34"/>
+      <c r="E344" s="34"/>
+      <c r="F344" s="20"/>
+      <c r="G344" s="20"/>
+      <c r="H344" s="20"/>
+    </row>
+    <row r="345" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C345" s="34"/>
+      <c r="D345" s="34"/>
+      <c r="E345" s="34"/>
+      <c r="F345" s="20"/>
+      <c r="G345" s="20"/>
+      <c r="H345" s="20"/>
+    </row>
+    <row r="346" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C346" s="34"/>
+      <c r="D346" s="34"/>
+      <c r="E346" s="34"/>
+      <c r="F346" s="20"/>
+      <c r="G346" s="20"/>
+      <c r="H346" s="20"/>
+    </row>
+    <row r="347" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C347" s="34"/>
+      <c r="D347" s="34"/>
+      <c r="E347" s="34"/>
+      <c r="F347" s="20"/>
+      <c r="G347" s="20"/>
+      <c r="H347" s="20"/>
+    </row>
+    <row r="348" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C348" s="34"/>
+      <c r="D348" s="34"/>
+      <c r="E348" s="34"/>
+      <c r="F348" s="20"/>
+      <c r="G348" s="20"/>
+      <c r="H348" s="20"/>
+    </row>
+    <row r="349" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C349" s="34"/>
+      <c r="D349" s="34"/>
+      <c r="E349" s="34"/>
+      <c r="F349" s="20"/>
+      <c r="G349" s="20"/>
+      <c r="H349" s="20"/>
+    </row>
+    <row r="350" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C350" s="34"/>
+      <c r="D350" s="34"/>
+      <c r="E350" s="34"/>
+      <c r="F350" s="20"/>
+      <c r="G350" s="20"/>
+      <c r="H350" s="20"/>
+    </row>
+    <row r="351" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C351" s="34"/>
+      <c r="D351" s="34"/>
+      <c r="E351" s="34"/>
+      <c r="F351" s="20"/>
+      <c r="G351" s="20"/>
+      <c r="H351" s="20"/>
+    </row>
+    <row r="352" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C352" s="34"/>
+      <c r="D352" s="34"/>
+      <c r="E352" s="34"/>
+      <c r="F352" s="20"/>
+      <c r="G352" s="20"/>
+      <c r="H352" s="20"/>
+    </row>
+    <row r="353" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C353" s="34"/>
+      <c r="D353" s="34"/>
+      <c r="E353" s="34"/>
+      <c r="F353" s="20"/>
+      <c r="G353" s="20"/>
+      <c r="H353" s="20"/>
+    </row>
+    <row r="354" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C354" s="34"/>
+      <c r="D354" s="34"/>
+      <c r="E354" s="34"/>
+      <c r="F354" s="20"/>
+      <c r="G354" s="20"/>
+      <c r="H354" s="20"/>
+    </row>
+    <row r="355" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C355" s="34"/>
+      <c r="D355" s="34"/>
+      <c r="E355" s="34"/>
+      <c r="F355" s="20"/>
+      <c r="G355" s="20"/>
+      <c r="H355" s="20"/>
+    </row>
+    <row r="356" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C356" s="34"/>
+      <c r="D356" s="34"/>
+      <c r="E356" s="34"/>
+      <c r="F356" s="20"/>
+      <c r="G356" s="20"/>
+      <c r="H356" s="20"/>
+    </row>
+    <row r="357" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C357" s="34"/>
+      <c r="D357" s="34"/>
+      <c r="E357" s="34"/>
+      <c r="F357" s="20"/>
+      <c r="G357" s="20"/>
+      <c r="H357" s="20"/>
+    </row>
+    <row r="358" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C358" s="34"/>
+      <c r="D358" s="34"/>
+      <c r="E358" s="34"/>
+      <c r="F358" s="20"/>
+      <c r="G358" s="20"/>
+      <c r="H358" s="20"/>
+    </row>
+    <row r="359" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C359" s="34"/>
+      <c r="D359" s="34"/>
+      <c r="E359" s="34"/>
+      <c r="F359" s="20"/>
+      <c r="G359" s="20"/>
+      <c r="H359" s="20"/>
+    </row>
+    <row r="360" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C360" s="34"/>
+      <c r="D360" s="34"/>
+      <c r="E360" s="34"/>
+      <c r="F360" s="20"/>
+      <c r="G360" s="20"/>
+      <c r="H360" s="20"/>
+    </row>
+    <row r="361" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C361" s="34"/>
+      <c r="D361" s="34"/>
+      <c r="E361" s="34"/>
+      <c r="F361" s="20"/>
+      <c r="G361" s="20"/>
+      <c r="H361" s="20"/>
+    </row>
+    <row r="362" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C362" s="34"/>
+      <c r="D362" s="34"/>
+      <c r="E362" s="34"/>
+      <c r="F362" s="20"/>
+      <c r="G362" s="20"/>
+      <c r="H362" s="20"/>
+    </row>
+    <row r="363" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C363" s="34"/>
+      <c r="D363" s="34"/>
+      <c r="E363" s="34"/>
+      <c r="F363" s="20"/>
+      <c r="G363" s="20"/>
+      <c r="H363" s="20"/>
+    </row>
+    <row r="364" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C364" s="34"/>
+      <c r="D364" s="34"/>
+      <c r="E364" s="34"/>
+      <c r="F364" s="20"/>
+      <c r="G364" s="20"/>
+      <c r="H364" s="20"/>
+    </row>
+    <row r="365" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C365" s="34"/>
+      <c r="D365" s="34"/>
+      <c r="E365" s="34"/>
+      <c r="F365" s="20"/>
+      <c r="G365" s="20"/>
+      <c r="H365" s="20"/>
+    </row>
+    <row r="366" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C366" s="34"/>
+      <c r="D366" s="34"/>
+      <c r="E366" s="34"/>
+      <c r="F366" s="20"/>
+      <c r="G366" s="20"/>
+      <c r="H366" s="20"/>
+    </row>
+    <row r="367" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C367" s="34"/>
+      <c r="D367" s="34"/>
+      <c r="E367" s="34"/>
+      <c r="F367" s="20"/>
+      <c r="G367" s="20"/>
+      <c r="H367" s="20"/>
+    </row>
+    <row r="368" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C368" s="34"/>
+      <c r="D368" s="34"/>
+      <c r="E368" s="34"/>
+      <c r="F368" s="20"/>
+      <c r="G368" s="20"/>
+      <c r="H368" s="20"/>
+    </row>
+    <row r="369" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C369" s="34"/>
+      <c r="D369" s="34"/>
+      <c r="E369" s="34"/>
+      <c r="F369" s="20"/>
+      <c r="G369" s="20"/>
+      <c r="H369" s="20"/>
+    </row>
+    <row r="370" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C370" s="34"/>
+      <c r="D370" s="34"/>
+      <c r="E370" s="34"/>
+      <c r="F370" s="20"/>
+      <c r="G370" s="20"/>
+      <c r="H370" s="20"/>
+    </row>
+    <row r="371" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C371" s="34"/>
+      <c r="D371" s="34"/>
+      <c r="E371" s="34"/>
+      <c r="F371" s="20"/>
+      <c r="G371" s="20"/>
+      <c r="H371" s="20"/>
+    </row>
+    <row r="372" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C372" s="34"/>
+      <c r="D372" s="34"/>
+      <c r="E372" s="34"/>
+      <c r="F372" s="20"/>
+      <c r="G372" s="20"/>
+      <c r="H372" s="20"/>
+    </row>
+    <row r="373" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C373" s="34"/>
+      <c r="D373" s="34"/>
+      <c r="E373" s="34"/>
+      <c r="F373" s="20"/>
+      <c r="G373" s="20"/>
+      <c r="H373" s="20"/>
+    </row>
+    <row r="374" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C374" s="34"/>
+      <c r="D374" s="34"/>
+      <c r="E374" s="34"/>
+      <c r="F374" s="20"/>
+      <c r="G374" s="20"/>
+      <c r="H374" s="20"/>
+    </row>
+    <row r="375" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C375" s="34"/>
+      <c r="D375" s="34"/>
+      <c r="E375" s="34"/>
+      <c r="F375" s="20"/>
+      <c r="G375" s="20"/>
+      <c r="H375" s="20"/>
+    </row>
+    <row r="376" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C376" s="34"/>
+      <c r="D376" s="34"/>
+      <c r="E376" s="34"/>
+      <c r="F376" s="20"/>
+      <c r="G376" s="20"/>
+      <c r="H376" s="20"/>
+    </row>
+    <row r="377" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C377" s="34"/>
+      <c r="D377" s="34"/>
+      <c r="E377" s="34"/>
+      <c r="F377" s="20"/>
+      <c r="G377" s="20"/>
+      <c r="H377" s="20"/>
+    </row>
+    <row r="378" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C378" s="34"/>
+      <c r="D378" s="34"/>
+      <c r="E378" s="34"/>
+      <c r="F378" s="20"/>
+      <c r="G378" s="20"/>
+      <c r="H378" s="20"/>
+    </row>
+    <row r="379" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C379" s="34"/>
+      <c r="D379" s="34"/>
+      <c r="E379" s="34"/>
+      <c r="F379" s="20"/>
+      <c r="G379" s="20"/>
+      <c r="H379" s="20"/>
+    </row>
+    <row r="380" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C380" s="34"/>
+      <c r="D380" s="34"/>
+      <c r="E380" s="34"/>
+      <c r="F380" s="20"/>
+      <c r="G380" s="20"/>
+      <c r="H380" s="20"/>
+    </row>
+    <row r="381" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C381" s="34"/>
+      <c r="D381" s="34"/>
+      <c r="E381" s="34"/>
+      <c r="F381" s="20"/>
+      <c r="G381" s="20"/>
+      <c r="H381" s="20"/>
+    </row>
+    <row r="382" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C382" s="34"/>
+      <c r="D382" s="34"/>
+      <c r="E382" s="34"/>
+      <c r="F382" s="20"/>
+      <c r="G382" s="20"/>
+      <c r="H382" s="20"/>
+    </row>
+    <row r="383" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C383" s="34"/>
+      <c r="D383" s="34"/>
+      <c r="E383" s="34"/>
+      <c r="F383" s="20"/>
+      <c r="G383" s="20"/>
+      <c r="H383" s="20"/>
+    </row>
+    <row r="384" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C384" s="34"/>
+      <c r="D384" s="34"/>
+      <c r="E384" s="34"/>
+      <c r="F384" s="20"/>
+      <c r="G384" s="20"/>
+      <c r="H384" s="20"/>
+    </row>
+    <row r="385" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C385" s="34"/>
+      <c r="D385" s="34"/>
+      <c r="E385" s="34"/>
+      <c r="F385" s="20"/>
+      <c r="G385" s="20"/>
+      <c r="H385" s="20"/>
+    </row>
+    <row r="386" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C386" s="34"/>
+      <c r="D386" s="34"/>
+      <c r="E386" s="34"/>
+      <c r="F386" s="20"/>
+      <c r="G386" s="20"/>
+      <c r="H386" s="20"/>
+    </row>
+    <row r="387" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C387" s="34"/>
+      <c r="D387" s="34"/>
+      <c r="E387" s="34"/>
+      <c r="F387" s="20"/>
+      <c r="G387" s="20"/>
+      <c r="H387" s="20"/>
+    </row>
+    <row r="388" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C388" s="34"/>
+      <c r="D388" s="34"/>
+      <c r="E388" s="34"/>
+      <c r="F388" s="20"/>
+      <c r="G388" s="20"/>
+      <c r="H388" s="20"/>
+    </row>
+    <row r="389" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C389" s="34"/>
+      <c r="D389" s="34"/>
+      <c r="E389" s="34"/>
+      <c r="F389" s="20"/>
+      <c r="G389" s="20"/>
+      <c r="H389" s="20"/>
+    </row>
+    <row r="390" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C390" s="34"/>
+      <c r="D390" s="34"/>
+      <c r="E390" s="34"/>
+      <c r="F390" s="20"/>
+      <c r="G390" s="20"/>
+      <c r="H390" s="20"/>
+    </row>
+    <row r="391" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C391" s="34"/>
+      <c r="D391" s="34"/>
+      <c r="E391" s="34"/>
+      <c r="F391" s="20"/>
+      <c r="G391" s="20"/>
+      <c r="H391" s="20"/>
+    </row>
+    <row r="392" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C392" s="34"/>
+      <c r="D392" s="34"/>
+      <c r="E392" s="34"/>
+      <c r="F392" s="20"/>
+      <c r="G392" s="20"/>
+      <c r="H392" s="20"/>
+    </row>
+    <row r="393" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C393" s="34"/>
+      <c r="D393" s="34"/>
+      <c r="E393" s="34"/>
+      <c r="F393" s="20"/>
+      <c r="G393" s="20"/>
+      <c r="H393" s="20"/>
+    </row>
+    <row r="394" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C394" s="34"/>
+      <c r="D394" s="34"/>
+      <c r="E394" s="34"/>
+      <c r="F394" s="20"/>
+      <c r="G394" s="20"/>
+      <c r="H394" s="20"/>
+    </row>
+    <row r="395" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C395" s="34"/>
+      <c r="D395" s="34"/>
+      <c r="E395" s="34"/>
+      <c r="F395" s="20"/>
+      <c r="G395" s="20"/>
+      <c r="H395" s="20"/>
+    </row>
+    <row r="396" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C396" s="34"/>
+      <c r="D396" s="34"/>
+      <c r="E396" s="34"/>
+      <c r="F396" s="20"/>
+      <c r="G396" s="20"/>
+      <c r="H396" s="20"/>
+    </row>
+    <row r="397" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C397" s="34"/>
+      <c r="D397" s="34"/>
+      <c r="E397" s="34"/>
+      <c r="F397" s="20"/>
+      <c r="G397" s="20"/>
+      <c r="H397" s="20"/>
+    </row>
+    <row r="398" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C398" s="34"/>
+      <c r="D398" s="34"/>
+      <c r="E398" s="34"/>
+      <c r="F398" s="20"/>
+      <c r="G398" s="20"/>
+      <c r="H398" s="20"/>
+    </row>
+    <row r="399" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C399" s="34"/>
+      <c r="D399" s="34"/>
+      <c r="E399" s="34"/>
+      <c r="F399" s="20"/>
+      <c r="G399" s="20"/>
+      <c r="H399" s="20"/>
+    </row>
+    <row r="400" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C400" s="34"/>
+      <c r="D400" s="34"/>
+      <c r="E400" s="34"/>
+      <c r="F400" s="20"/>
+      <c r="G400" s="20"/>
+      <c r="H400" s="20"/>
+    </row>
+    <row r="401" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C401" s="34"/>
+      <c r="D401" s="34"/>
+      <c r="E401" s="34"/>
+      <c r="F401" s="20"/>
+      <c r="G401" s="20"/>
+      <c r="H401" s="20"/>
+    </row>
+    <row r="402" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C402" s="34"/>
+      <c r="D402" s="34"/>
+      <c r="E402" s="34"/>
+      <c r="F402" s="20"/>
+      <c r="G402" s="20"/>
+      <c r="H402" s="20"/>
+    </row>
+    <row r="403" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C403" s="34"/>
+      <c r="D403" s="34"/>
+      <c r="E403" s="34"/>
+      <c r="F403" s="20"/>
+      <c r="G403" s="20"/>
+      <c r="H403" s="20"/>
+    </row>
+    <row r="404" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C404" s="34"/>
+      <c r="D404" s="34"/>
+      <c r="E404" s="34"/>
+      <c r="F404" s="20"/>
+      <c r="G404" s="20"/>
+      <c r="H404" s="20"/>
+    </row>
+    <row r="405" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C405" s="34"/>
+      <c r="D405" s="34"/>
+      <c r="E405" s="34"/>
+      <c r="F405" s="20"/>
+      <c r="G405" s="20"/>
+      <c r="H405" s="20"/>
+    </row>
+    <row r="406" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C406" s="34"/>
+      <c r="D406" s="34"/>
+      <c r="E406" s="34"/>
+      <c r="F406" s="20"/>
+      <c r="G406" s="20"/>
+      <c r="H406" s="20"/>
+    </row>
+    <row r="407" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C407" s="34"/>
+      <c r="D407" s="34"/>
+      <c r="E407" s="34"/>
+      <c r="F407" s="20"/>
+      <c r="G407" s="20"/>
+      <c r="H407" s="20"/>
+    </row>
+    <row r="408" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C408" s="34"/>
+      <c r="D408" s="34"/>
+      <c r="E408" s="34"/>
+      <c r="F408" s="20"/>
+      <c r="G408" s="20"/>
+      <c r="H408" s="20"/>
+    </row>
+    <row r="409" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C409" s="34"/>
+      <c r="D409" s="34"/>
+      <c r="E409" s="34"/>
+      <c r="F409" s="20"/>
+      <c r="G409" s="20"/>
+      <c r="H409" s="20"/>
+    </row>
+    <row r="410" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C410" s="34"/>
+      <c r="D410" s="34"/>
+      <c r="E410" s="34"/>
+      <c r="F410" s="20"/>
+      <c r="G410" s="20"/>
+      <c r="H410" s="20"/>
+    </row>
+    <row r="411" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C411" s="34"/>
+      <c r="D411" s="34"/>
+      <c r="E411" s="34"/>
+      <c r="F411" s="20"/>
+      <c r="G411" s="20"/>
+      <c r="H411" s="20"/>
+    </row>
+    <row r="412" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C412" s="34"/>
+      <c r="D412" s="34"/>
+      <c r="E412" s="34"/>
+      <c r="F412" s="20"/>
+      <c r="G412" s="20"/>
+      <c r="H412" s="20"/>
+    </row>
+    <row r="413" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C413" s="34"/>
+      <c r="D413" s="34"/>
+      <c r="E413" s="34"/>
+      <c r="F413" s="20"/>
+      <c r="G413" s="20"/>
+      <c r="H413" s="20"/>
+    </row>
+    <row r="414" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C414" s="34"/>
+      <c r="D414" s="34"/>
+      <c r="E414" s="34"/>
+      <c r="F414" s="20"/>
+      <c r="G414" s="20"/>
+      <c r="H414" s="20"/>
+    </row>
+    <row r="415" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C415" s="34"/>
+      <c r="D415" s="34"/>
+      <c r="E415" s="34"/>
+      <c r="F415" s="20"/>
+      <c r="G415" s="20"/>
+      <c r="H415" s="20"/>
+    </row>
+    <row r="416" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C416" s="34"/>
+      <c r="D416" s="34"/>
+      <c r="E416" s="34"/>
+      <c r="F416" s="20"/>
+      <c r="G416" s="20"/>
+      <c r="H416" s="20"/>
+    </row>
+    <row r="417" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C417" s="34"/>
+      <c r="D417" s="34"/>
+      <c r="E417" s="34"/>
+      <c r="F417" s="20"/>
+      <c r="G417" s="20"/>
+      <c r="H417" s="20"/>
+    </row>
+    <row r="418" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C418" s="34"/>
+      <c r="D418" s="34"/>
+      <c r="E418" s="34"/>
+      <c r="F418" s="20"/>
+      <c r="G418" s="20"/>
+      <c r="H418" s="20"/>
+    </row>
+    <row r="419" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C419" s="34"/>
+      <c r="D419" s="34"/>
+      <c r="E419" s="34"/>
+      <c r="F419" s="20"/>
+      <c r="G419" s="20"/>
+      <c r="H419" s="20"/>
+    </row>
+    <row r="420" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C420" s="34"/>
+      <c r="D420" s="34"/>
+      <c r="E420" s="34"/>
+      <c r="F420" s="20"/>
+      <c r="G420" s="20"/>
+      <c r="H420" s="20"/>
+    </row>
+    <row r="421" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C421" s="34"/>
+      <c r="D421" s="34"/>
+      <c r="E421" s="34"/>
+      <c r="F421" s="20"/>
+      <c r="G421" s="20"/>
+      <c r="H421" s="20"/>
+    </row>
+    <row r="422" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C422" s="34"/>
+      <c r="D422" s="34"/>
+      <c r="E422" s="34"/>
+      <c r="F422" s="20"/>
+      <c r="G422" s="20"/>
+      <c r="H422" s="20"/>
+    </row>
+    <row r="423" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C423" s="34"/>
+      <c r="D423" s="34"/>
+      <c r="E423" s="34"/>
+      <c r="F423" s="20"/>
+      <c r="G423" s="20"/>
+      <c r="H423" s="20"/>
+    </row>
+    <row r="424" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C424" s="34"/>
+      <c r="D424" s="34"/>
+      <c r="E424" s="34"/>
+      <c r="F424" s="20"/>
+      <c r="G424" s="20"/>
+      <c r="H424" s="20"/>
+    </row>
+    <row r="425" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C425" s="34"/>
+      <c r="D425" s="34"/>
+      <c r="E425" s="34"/>
+      <c r="F425" s="20"/>
+      <c r="G425" s="20"/>
+      <c r="H425" s="20"/>
+    </row>
+    <row r="426" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C426" s="34"/>
+      <c r="D426" s="34"/>
+      <c r="E426" s="34"/>
+      <c r="F426" s="20"/>
+      <c r="G426" s="20"/>
+      <c r="H426" s="20"/>
+    </row>
+    <row r="427" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C427" s="34"/>
+      <c r="D427" s="34"/>
+      <c r="E427" s="34"/>
+      <c r="F427" s="20"/>
+      <c r="G427" s="20"/>
+      <c r="H427" s="20"/>
+    </row>
+    <row r="428" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C428" s="34"/>
+      <c r="D428" s="34"/>
+      <c r="E428" s="34"/>
+      <c r="F428" s="20"/>
+      <c r="G428" s="20"/>
+      <c r="H428" s="20"/>
+    </row>
+    <row r="429" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C429" s="34"/>
+      <c r="D429" s="34"/>
+      <c r="E429" s="34"/>
+      <c r="F429" s="20"/>
+      <c r="G429" s="20"/>
+      <c r="H429" s="20"/>
+    </row>
+    <row r="430" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C430" s="34"/>
+      <c r="D430" s="34"/>
+      <c r="E430" s="34"/>
+      <c r="F430" s="20"/>
+      <c r="G430" s="20"/>
+      <c r="H430" s="20"/>
+    </row>
+    <row r="431" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C431" s="34"/>
+      <c r="D431" s="34"/>
+      <c r="E431" s="34"/>
+      <c r="F431" s="20"/>
+      <c r="G431" s="20"/>
+      <c r="H431" s="20"/>
+    </row>
+    <row r="432" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C432" s="34"/>
+      <c r="D432" s="34"/>
+      <c r="E432" s="34"/>
+      <c r="F432" s="20"/>
+      <c r="G432" s="20"/>
+      <c r="H432" s="20"/>
+    </row>
+    <row r="433" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C433" s="34"/>
+      <c r="D433" s="34"/>
+      <c r="E433" s="34"/>
+      <c r="F433" s="20"/>
+      <c r="G433" s="20"/>
+      <c r="H433" s="20"/>
+    </row>
+    <row r="434" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C434" s="34"/>
+      <c r="D434" s="34"/>
+      <c r="E434" s="34"/>
+      <c r="F434" s="20"/>
+      <c r="G434" s="20"/>
+      <c r="H434" s="20"/>
+    </row>
+    <row r="435" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C435" s="34"/>
+      <c r="D435" s="34"/>
+      <c r="E435" s="34"/>
+      <c r="F435" s="20"/>
+      <c r="G435" s="20"/>
+      <c r="H435" s="20"/>
+    </row>
+    <row r="436" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C436" s="34"/>
+      <c r="D436" s="34"/>
+      <c r="E436" s="34"/>
+      <c r="F436" s="20"/>
+      <c r="G436" s="20"/>
+      <c r="H436" s="20"/>
+    </row>
+    <row r="437" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C437" s="34"/>
+      <c r="D437" s="34"/>
+      <c r="E437" s="34"/>
+      <c r="F437" s="20"/>
+      <c r="G437" s="20"/>
+      <c r="H437" s="20"/>
+    </row>
+    <row r="438" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C438" s="34"/>
+      <c r="D438" s="34"/>
+      <c r="E438" s="34"/>
+      <c r="F438" s="20"/>
+      <c r="G438" s="20"/>
+      <c r="H438" s="20"/>
+    </row>
+    <row r="439" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C439" s="34"/>
+      <c r="D439" s="34"/>
+      <c r="E439" s="34"/>
+      <c r="F439" s="20"/>
+      <c r="G439" s="20"/>
+      <c r="H439" s="20"/>
+    </row>
+    <row r="440" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C440" s="34"/>
+      <c r="D440" s="34"/>
+      <c r="E440" s="34"/>
+      <c r="F440" s="20"/>
+      <c r="G440" s="20"/>
+      <c r="H440" s="20"/>
+    </row>
+    <row r="441" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C441" s="34"/>
+      <c r="D441" s="34"/>
+      <c r="E441" s="34"/>
+      <c r="F441" s="20"/>
+      <c r="G441" s="20"/>
+      <c r="H441" s="20"/>
+    </row>
+    <row r="442" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C442" s="34"/>
+      <c r="D442" s="34"/>
+      <c r="E442" s="34"/>
+      <c r="F442" s="20"/>
+      <c r="G442" s="20"/>
+      <c r="H442" s="20"/>
+    </row>
+    <row r="443" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C443" s="34"/>
+      <c r="D443" s="34"/>
+      <c r="E443" s="34"/>
+      <c r="F443" s="20"/>
+      <c r="G443" s="20"/>
+      <c r="H443" s="20"/>
+    </row>
+    <row r="444" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C444" s="34"/>
+      <c r="D444" s="34"/>
+      <c r="E444" s="34"/>
+      <c r="F444" s="20"/>
+      <c r="G444" s="20"/>
+      <c r="H444" s="20"/>
+    </row>
+    <row r="445" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C445" s="34"/>
+      <c r="D445" s="34"/>
+      <c r="E445" s="34"/>
+      <c r="F445" s="20"/>
+      <c r="G445" s="20"/>
+      <c r="H445" s="20"/>
+    </row>
+    <row r="446" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C446" s="34"/>
+      <c r="D446" s="34"/>
+      <c r="E446" s="34"/>
+      <c r="F446" s="20"/>
+      <c r="G446" s="20"/>
+      <c r="H446" s="20"/>
+    </row>
+    <row r="447" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C447" s="34"/>
+      <c r="D447" s="34"/>
+      <c r="E447" s="34"/>
+      <c r="F447" s="20"/>
+      <c r="G447" s="20"/>
+      <c r="H447" s="20"/>
+    </row>
+    <row r="448" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C448" s="34"/>
+      <c r="D448" s="34"/>
+      <c r="E448" s="34"/>
+      <c r="F448" s="20"/>
+      <c r="G448" s="20"/>
+      <c r="H448" s="20"/>
+    </row>
+    <row r="449" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C449" s="34"/>
+      <c r="D449" s="34"/>
+      <c r="E449" s="34"/>
+      <c r="F449" s="20"/>
+      <c r="G449" s="20"/>
+      <c r="H449" s="20"/>
+    </row>
+    <row r="450" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C450" s="34"/>
+      <c r="D450" s="34"/>
+      <c r="E450" s="34"/>
+      <c r="F450" s="20"/>
+      <c r="G450" s="20"/>
+      <c r="H450" s="20"/>
+    </row>
+    <row r="451" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C451" s="34"/>
+      <c r="D451" s="34"/>
+      <c r="E451" s="34"/>
+      <c r="F451" s="20"/>
+      <c r="G451" s="20"/>
+      <c r="H451" s="20"/>
+    </row>
+    <row r="452" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C452" s="34"/>
+      <c r="D452" s="34"/>
+      <c r="E452" s="34"/>
+      <c r="F452" s="20"/>
+      <c r="G452" s="20"/>
+      <c r="H452" s="20"/>
+    </row>
+    <row r="453" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C453" s="34"/>
+      <c r="D453" s="34"/>
+      <c r="E453" s="34"/>
+      <c r="F453" s="20"/>
+      <c r="G453" s="20"/>
+      <c r="H453" s="20"/>
+    </row>
+    <row r="454" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C454" s="34"/>
+      <c r="D454" s="34"/>
+      <c r="E454" s="34"/>
+      <c r="F454" s="20"/>
+      <c r="G454" s="20"/>
+      <c r="H454" s="20"/>
+    </row>
+    <row r="455" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C455" s="34"/>
+      <c r="D455" s="34"/>
+      <c r="E455" s="34"/>
+      <c r="F455" s="20"/>
+      <c r="G455" s="20"/>
+      <c r="H455" s="20"/>
+    </row>
+    <row r="456" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C456" s="34"/>
+      <c r="D456" s="34"/>
+      <c r="E456" s="34"/>
+      <c r="F456" s="20"/>
+      <c r="G456" s="20"/>
+      <c r="H456" s="20"/>
+    </row>
+    <row r="457" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C457" s="34"/>
+      <c r="D457" s="34"/>
+      <c r="E457" s="34"/>
+      <c r="F457" s="20"/>
+      <c r="G457" s="20"/>
+      <c r="H457" s="20"/>
+    </row>
+    <row r="458" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C458" s="34"/>
+      <c r="D458" s="34"/>
+      <c r="E458" s="34"/>
+      <c r="F458" s="20"/>
+      <c r="G458" s="20"/>
+      <c r="H458" s="20"/>
+    </row>
+    <row r="459" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C459" s="34"/>
+      <c r="D459" s="34"/>
+      <c r="E459" s="34"/>
+      <c r="F459" s="20"/>
+      <c r="G459" s="20"/>
+      <c r="H459" s="20"/>
+    </row>
+    <row r="460" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C460" s="34"/>
+      <c r="D460" s="34"/>
+      <c r="E460" s="34"/>
+      <c r="F460" s="20"/>
+      <c r="G460" s="20"/>
+      <c r="H460" s="20"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41393E51-CA3C-4A23-9C04-919BFB576ADB}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -2692,10 +6465,10 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30"/>
+      <c r="B2" s="32"/>
       <c r="C2" s="2" t="s">
         <v>14</v>
       </c>
@@ -2773,7 +6546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68574BDA-3780-4F30-ACB9-BC66FA2B1114}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
@@ -2781,7 +6554,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2843,13 +6616,22 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C12" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="33">
+        <f>SUM(D3:D11)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <f>SUM(E3:E11)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D13" s="13"/>
@@ -2873,7 +6655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B55ED5B-4EDE-43B1-AA7B-733BBABD30C8}">
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>

</xml_diff>

<commit_message>
update template to calculate dividend per capita
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damon\OneDrive\Documents\GitLab\SPECTRUM\Projects\smoke-free-dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C0556-9D83-4C87-884B-167E09A88F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82375A5C-0744-458D-9AC1-786F9B864105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="7" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="6" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="114">
   <si>
     <t>All</t>
   </si>
@@ -476,6 +476,12 @@
   <si>
     <t>* Local authorities with fewer than 10 observations are excluded.</t>
   </si>
+  <si>
+    <t>18+ Population</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dividend per capita (£m) </t>
+  </si>
 </sst>
 </file>
 
@@ -687,7 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -800,6 +806,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -842,9 +851,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1181,27 +1192,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71" t="s">
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
       <c r="H3" s="13" t="s">
         <v>36</v>
       </c>
@@ -1342,15 +1353,15 @@
       <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="70" t="s">
+      <c r="B15" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="70"/>
-      <c r="H15" s="70"/>
+      <c r="C15" s="71"/>
+      <c r="D15" s="71"/>
+      <c r="E15" s="71"/>
+      <c r="F15" s="71"/>
+      <c r="G15" s="71"/>
+      <c r="H15" s="71"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1416,22 +1427,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="72" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="72"/>
-      <c r="H1" s="74" t="s">
+      <c r="G1" s="73"/>
+      <c r="H1" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="74"/>
-      <c r="J1" s="74"/>
-      <c r="K1" s="74"/>
-      <c r="L1" s="74"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
@@ -3987,7 +3998,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4013,12 +4024,12 @@
       <c r="E1" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="75" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="74"/>
-      <c r="H1" s="74"/>
-      <c r="I1" s="74"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -5775,12 +5786,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="74" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
@@ -9705,12 +9716,12 @@
       <c r="E16" s="58"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="80" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
+      <c r="C17" s="80"/>
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
@@ -9735,61 +9746,61 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="80" t="str">
+      <c r="B21" s="81" t="str">
         <f>HYPERLINK("https://www.gov.uk/government/statistics/tobacco-bulletin", "(a) 2018/19 figures obtained from the HMRC July 2021 Tobacco Bulletin tables ")</f>
         <v xml:space="preserve">(a) 2018/19 figures obtained from the HMRC July 2021 Tobacco Bulletin tables </v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="81"/>
-      <c r="E21" s="81"/>
+      <c r="C21" s="82"/>
+      <c r="D21" s="82"/>
+      <c r="E21" s="82"/>
       <c r="F21" s="22"/>
     </row>
     <row r="22" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="75" t="str">
+      <c r="B22" s="76" t="str">
         <f>HYPERLINK("https://www.oecd.org/tax/consumption/tax-burden-cigarettes-ctt-trends.xlsx", "(b) OECD. Weighted Average Price in 2016 inflated to 2018 prices")</f>
         <v>(b) OECD. Weighted Average Price in 2016 inflated to 2018 prices</v>
       </c>
-      <c r="C22" s="76"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
+      <c r="C22" s="77"/>
+      <c r="D22" s="77"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="22"/>
     </row>
     <row r="23" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="75" t="str">
+      <c r="B23" s="76" t="str">
         <f>HYPERLINK("https://www.gov.uk/government/statistics/tobacco-bulletin/tobacco-duty-rates", "(c) Tobacco duty rates as of December 2018. HMRC Tobacco Bulletin")</f>
         <v>(c) Tobacco duty rates as of December 2018. HMRC Tobacco Bulletin</v>
       </c>
-      <c r="C23" s="76"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
+      <c r="C23" s="77"/>
+      <c r="D23" s="77"/>
+      <c r="E23" s="77"/>
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="82" t="s">
+      <c r="B24" s="83" t="s">
         <v>106</v>
       </c>
-      <c r="C24" s="82"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
+      <c r="C24" s="83"/>
+      <c r="D24" s="83"/>
+      <c r="E24" s="83"/>
     </row>
     <row r="25" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="75" t="str">
+      <c r="B25" s="76" t="str">
         <f>HYPERLINK("https://www.gov.uk/government/statistics/measuring-tax-gaps-tables", "(e) 2018/19 illicit consumption obtained from the HMRC Measuring tax gaps tables ")</f>
         <v xml:space="preserve">(e) 2018/19 illicit consumption obtained from the HMRC Measuring tax gaps tables </v>
       </c>
-      <c r="C25" s="76"/>
-      <c r="D25" s="76"/>
-      <c r="E25" s="76"/>
+      <c r="C25" s="77"/>
+      <c r="D25" s="77"/>
+      <c r="E25" s="77"/>
       <c r="F25" s="22"/>
     </row>
     <row r="26" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="77" t="str">
+      <c r="B26" s="78" t="str">
         <f>HYPERLINK("https://www.ashscotland.org.uk/media/850413/28-calculating-the-cost-of-smoking-june-2021.pdf", "(f) estimates of illicit tobacco product prices obtained from ASH Scotland ")</f>
         <v xml:space="preserve">(f) estimates of illicit tobacco product prices obtained from ASH Scotland </v>
       </c>
-      <c r="C26" s="78"/>
-      <c r="D26" s="78"/>
-      <c r="E26" s="78"/>
+      <c r="C26" s="79"/>
+      <c r="D26" s="79"/>
+      <c r="E26" s="79"/>
       <c r="F26" s="22"/>
     </row>
     <row r="27" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -9831,8 +9842,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="83"/>
-      <c r="B2" s="83"/>
+      <c r="A2" s="84"/>
+      <c r="B2" s="84"/>
       <c r="C2" s="40" t="s">
         <v>72</v>
       </c>
@@ -10007,10 +10018,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:G231"/>
+  <dimension ref="A1:J231"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10020,10 +10031,13 @@
     <col min="4" max="4" width="10.28515625" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="1" t="s">
         <v>85</v>
@@ -10034,7 +10048,7 @@
       <c r="F1" s="16"/>
       <c r="G1" s="16"/>
     </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" s="2" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="47" t="s">
         <v>10</v>
@@ -10054,8 +10068,17 @@
       <c r="G2" s="49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="86" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>'Region data'!$B3</f>
         <v>0</v>
@@ -10080,8 +10103,20 @@
         <f>'Region data'!$L3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="85">
+        <f>'Region data'!$F3/100</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="10" t="e">
+        <f>D3/H3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3" s="87" t="e">
+        <f>(G3*1000000)/I3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>'Region data'!$B4</f>
         <v>0</v>
@@ -10106,8 +10141,20 @@
         <f>'Region data'!$L4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="85">
+        <f>'Region data'!$F4/100</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="10" t="e">
+        <f t="shared" ref="I4:I11" si="0">D4/H4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4" s="87" t="e">
+        <f t="shared" ref="J4:J11" si="1">(G4*1000000)/I4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>'Region data'!$B5</f>
         <v>0</v>
@@ -10132,8 +10179,20 @@
         <f>'Region data'!$L5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="85">
+        <f>'Region data'!$F5/100</f>
+        <v>0</v>
+      </c>
+      <c r="I5" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>'Region data'!$B6</f>
         <v>0</v>
@@ -10158,8 +10217,20 @@
         <f>'Region data'!$L6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="85">
+        <f>'Region data'!$F6/100</f>
+        <v>0</v>
+      </c>
+      <c r="I6" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J6" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>'Region data'!$B7</f>
         <v>0</v>
@@ -10184,8 +10255,20 @@
         <f>'Region data'!$L7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="85">
+        <f>'Region data'!$F7/100</f>
+        <v>0</v>
+      </c>
+      <c r="I7" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J7" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>'Region data'!$B8</f>
         <v>0</v>
@@ -10210,8 +10293,20 @@
         <f>'Region data'!$L8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="85">
+        <f>'Region data'!$F8/100</f>
+        <v>0</v>
+      </c>
+      <c r="I8" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J8" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9">
         <f>'Region data'!$B9</f>
@@ -10237,8 +10332,20 @@
         <f>'Region data'!$L9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="85">
+        <f>'Region data'!$F9/100</f>
+        <v>0</v>
+      </c>
+      <c r="I9" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J9" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10">
         <f>'Region data'!$B10</f>
@@ -10264,8 +10371,20 @@
         <f>'Region data'!$L10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="85">
+        <f>'Region data'!$F10/100</f>
+        <v>0</v>
+      </c>
+      <c r="I10" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J10" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11">
         <f>'Region data'!$B11</f>
@@ -10291,15 +10410,28 @@
         <f>'Region data'!$L11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="85">
+        <f>'Region data'!$F11/100</f>
+        <v>0</v>
+      </c>
+      <c r="I11" s="10" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J11" s="87" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="C12" s="38"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I12" s="10"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -10316,16 +10448,22 @@
         <f>SUM(G3:G11)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13" s="37"/>
+      <c r="I13" s="36" t="e">
+        <f t="shared" ref="H13:J13" si="2">SUM(I3:I11)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J13" s="37"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="E16" s="11"/>
     </row>
@@ -10987,7 +11125,7 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -11104,7 +11242,7 @@
       <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="70" t="s">
         <v>111</v>
       </c>
       <c r="F13" s="12"/>
@@ -11257,7 +11395,7 @@
       <c r="G12" s="53"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="84" t="s">
+      <c r="B13" s="70" t="s">
         <v>111</v>
       </c>
       <c r="F13" s="12"/>

</xml_diff>

<commit_message>
add dividend per capita to the output tables
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damon\OneDrive\Documents\GitLab\SPECTRUM\Projects\smoke-free-dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FFD3BF-E27A-48DA-99EA-7FD44AEDE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C87B18B-2093-46DE-9067-2512CB27BCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="6" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="7" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="117">
   <si>
     <t>All</t>
   </si>
@@ -480,13 +480,16 @@
     <t>18+ Population</t>
   </si>
   <si>
-    <t xml:space="preserve"> Dividend per capita (£m) </t>
-  </si>
-  <si>
     <t>Weekly Spend per smoker (£)</t>
   </si>
   <si>
     <t>Weekly Income</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dividend per capita</t>
+  </si>
+  <si>
+    <t>Dividend per capita</t>
   </si>
 </sst>
 </file>
@@ -10024,8 +10027,8 @@
   </sheetPr>
   <dimension ref="A1:K231"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10059,7 +10062,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D2" s="48" t="s">
         <v>57</v>
@@ -10068,7 +10071,7 @@
         <v>64</v>
       </c>
       <c r="F2" s="48" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G2" s="48" t="s">
         <v>66</v>
@@ -10083,7 +10086,7 @@
         <v>112</v>
       </c>
       <c r="K2" s="49" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -11390,10 +11393,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11405,15 +11408,16 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>109</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>68</v>
       </c>
@@ -11435,71 +11439,83 @@
       <c r="G2" s="54" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="19"/>
       <c r="D3" s="38"/>
       <c r="E3" s="19"/>
       <c r="F3" s="9"/>
       <c r="G3" s="52"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="19"/>
       <c r="D4" s="38"/>
       <c r="E4" s="19"/>
       <c r="F4" s="9"/>
       <c r="G4" s="52"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="19"/>
       <c r="D5" s="38"/>
       <c r="E5" s="19"/>
       <c r="F5" s="9"/>
       <c r="G5" s="52"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="19"/>
       <c r="D6" s="38"/>
       <c r="E6" s="19"/>
       <c r="F6" s="9"/>
       <c r="G6" s="52"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="19"/>
       <c r="D7" s="38"/>
       <c r="E7" s="19"/>
       <c r="F7" s="9"/>
       <c r="G7" s="52"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="19"/>
       <c r="D8" s="38"/>
       <c r="E8" s="19"/>
       <c r="F8" s="9"/>
       <c r="G8" s="52"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="19"/>
       <c r="D9" s="38"/>
       <c r="E9" s="19"/>
       <c r="F9" s="9"/>
       <c r="G9" s="52"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="19"/>
       <c r="D10" s="38"/>
       <c r="E10" s="19"/>
       <c r="F10" s="9"/>
       <c r="G10" s="52"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="19"/>
       <c r="D11" s="38"/>
       <c r="E11" s="19"/>
       <c r="F11" s="9"/>
       <c r="G11" s="52"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
       <c r="C12" s="50"/>
@@ -11507,23 +11523,24 @@
       <c r="E12" s="50"/>
       <c r="F12" s="51"/>
       <c r="G12" s="53"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="51"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="70" t="s">
         <v>111</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>
@@ -11542,10 +11559,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="H3" sqref="H3:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11557,16 +11574,17 @@
     <col min="5" max="5" width="14" customWidth="1"/>
     <col min="6" max="6" width="17.28515625" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>110</v>
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="54" t="s">
         <v>68</v>
       </c>
@@ -11588,71 +11606,83 @@
       <c r="G2" s="54" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2" s="54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" s="19"/>
       <c r="D3" s="38"/>
       <c r="E3" s="19"/>
       <c r="F3" s="9"/>
       <c r="G3" s="52"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" s="19"/>
       <c r="D4" s="38"/>
       <c r="E4" s="19"/>
       <c r="F4" s="9"/>
       <c r="G4" s="52"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" s="19"/>
       <c r="D5" s="38"/>
       <c r="E5" s="19"/>
       <c r="F5" s="9"/>
       <c r="G5" s="52"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5" s="9"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C6" s="19"/>
       <c r="D6" s="38"/>
       <c r="E6" s="19"/>
       <c r="F6" s="9"/>
       <c r="G6" s="52"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C7" s="19"/>
       <c r="D7" s="38"/>
       <c r="E7" s="19"/>
       <c r="F7" s="9"/>
       <c r="G7" s="52"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C8" s="19"/>
       <c r="D8" s="38"/>
       <c r="E8" s="19"/>
       <c r="F8" s="9"/>
       <c r="G8" s="52"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8" s="9"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="19"/>
       <c r="D9" s="38"/>
       <c r="E9" s="19"/>
       <c r="F9" s="9"/>
       <c r="G9" s="52"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C10" s="19"/>
       <c r="D10" s="38"/>
       <c r="E10" s="19"/>
       <c r="F10" s="9"/>
       <c r="G10" s="52"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C11" s="19"/>
       <c r="D11" s="38"/>
       <c r="E11" s="19"/>
       <c r="F11" s="9"/>
       <c r="G11" s="52"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11" s="9"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
       <c r="C12" s="50"/>
@@ -11660,23 +11690,24 @@
       <c r="E12" s="50"/>
       <c r="F12" s="51"/>
       <c r="G12" s="53"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12" s="51"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="70" t="s">
         <v>111</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="12"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F14" s="12"/>
       <c r="G14" s="12"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
     </row>

</xml_diff>

<commit_message>
update results tables template to update source on cigarette price
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damon\OneDrive\Documents\GitLab\SPECTRUM\Projects\smoke-free-dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C87B18B-2093-46DE-9067-2512CB27BCFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC33115D-B8AE-4C99-9E16-4F90CA22A9A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="7" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" activeTab="4" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
@@ -9508,8 +9508,8 @@
   </sheetPr>
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9764,8 +9764,8 @@
     </row>
     <row r="22" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="77" t="str">
-        <f>HYPERLINK("https://www.oecd.org/tax/consumption/tax-burden-cigarettes-ctt-trends.xlsx", "(b) OECD. Weighted Average Price in 2016 inflated to 2018 prices")</f>
-        <v>(b) OECD. Weighted Average Price in 2016 inflated to 2018 prices</v>
+        <f>HYPERLINK("https://ec.europa.eu/taxation_customs/tedb/taxDetails.html?id=4155/1546297200", "(b) European Commission. Weighted Average Price as of 2019/01/01")</f>
+        <v>(b) European Commission. Weighted Average Price as of 2019/01/01</v>
       </c>
       <c r="C22" s="78"/>
       <c r="D22" s="78"/>
@@ -11395,7 +11395,7 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update analysis with new upshift
</commit_message>
<xml_diff>
--- a/templates/results_template.xlsx
+++ b/templates/results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damon\OneDrive\Documents\GitLab\SPECTRUM\Projects\smoke-free-dividend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FA5645-D58E-41E0-A3DC-BC0BB2B0FE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CB2126-272F-470B-A443-63EA16CCF2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" firstSheet="1" activeTab="6" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="689" firstSheet="1" activeTab="4" xr2:uid="{878172EC-09E9-4A7D-B265-07C6D7EC199A}"/>
   </bookViews>
   <sheets>
     <sheet name="Upshift Calcs" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="122">
   <si>
     <t>All</t>
   </si>
@@ -500,6 +500,12 @@
   <si>
     <t>Table 2b. Spending in local authorities with the lowest expenditure as a fraction of income</t>
   </si>
+  <si>
+    <t>Dividend per smoker (£)</t>
+  </si>
+  <si>
+    <t>Dividend per smoker</t>
+  </si>
 </sst>
 </file>
 
@@ -711,7 +717,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -836,6 +842,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -878,30 +908,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1238,27 +1246,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="82" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75" t="s">
+      <c r="C3" s="83"/>
+      <c r="D3" s="83"/>
+      <c r="E3" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
+      <c r="F3" s="83"/>
+      <c r="G3" s="83"/>
       <c r="H3" s="13" t="s">
         <v>36</v>
       </c>
@@ -1399,15 +1407,15 @@
       <c r="H14" s="31"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="74" t="s">
+      <c r="B15" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74"/>
-      <c r="H15" s="74"/>
+      <c r="C15" s="82"/>
+      <c r="D15" s="82"/>
+      <c r="E15" s="82"/>
+      <c r="F15" s="82"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -1444,13 +1452,13 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:R464"/>
+  <dimension ref="A1:S464"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="G3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="G122" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N15" sqref="N15"/>
+      <selection pane="bottomRight" activeCell="O145" sqref="O145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,33 +1480,35 @@
     <col min="16" max="16" width="16.42578125" customWidth="1"/>
     <col min="17" max="17" width="11.28515625" customWidth="1"/>
     <col min="18" max="18" width="13.7109375" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="C1" s="77" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C1" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="76" t="s">
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="84" t="s">
         <v>67</v>
       </c>
-      <c r="G1" s="76"/>
-      <c r="H1" s="78" t="s">
+      <c r="G1" s="84"/>
+      <c r="H1" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
       <c r="O1" s="8"/>
       <c r="P1" s="8"/>
       <c r="Q1" s="8"/>
       <c r="R1" s="8"/>
-    </row>
-    <row r="2" spans="1:18" s="2" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S1" s="8"/>
+    </row>
+    <row r="2" spans="1:19" s="2" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
@@ -1553,8 +1563,11 @@
       <c r="R2" s="71" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S2" s="71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C3" s="38"/>
       <c r="F3" s="10"/>
       <c r="J3" s="10"/>
@@ -1569,8 +1582,12 @@
         <f>(P3*1000000)/J3</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S3" s="96" t="e">
+        <f>(P3*1000000)/J3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C4" s="38"/>
       <c r="F4" s="10"/>
       <c r="J4" s="10"/>
@@ -1585,8 +1602,12 @@
         <f t="shared" ref="R4:R67" si="1">(P4*1000000)/J4</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S4" s="96" t="e">
+        <f t="shared" ref="S4:S67" si="2">(P4*1000000)/J4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C5" s="38"/>
       <c r="F5" s="10"/>
       <c r="J5" s="10"/>
@@ -1601,8 +1622,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S5" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C6" s="38"/>
       <c r="F6" s="10"/>
       <c r="J6" s="10"/>
@@ -1617,8 +1642,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C7" s="38"/>
       <c r="F7" s="10"/>
       <c r="J7" s="10"/>
@@ -1633,8 +1662,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C8" s="38"/>
       <c r="F8" s="10"/>
       <c r="J8" s="10"/>
@@ -1649,8 +1682,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C9" s="38"/>
       <c r="F9" s="10"/>
       <c r="J9" s="10"/>
@@ -1665,8 +1702,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S9" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C10" s="38"/>
       <c r="F10" s="10"/>
       <c r="J10" s="10"/>
@@ -1681,8 +1722,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S10" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C11" s="38"/>
       <c r="F11" s="10"/>
       <c r="J11" s="10"/>
@@ -1697,8 +1742,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S11" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C12" s="38"/>
       <c r="F12" s="10"/>
       <c r="J12" s="10"/>
@@ -1713,8 +1762,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S12" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C13" s="38"/>
       <c r="F13" s="10"/>
       <c r="J13" s="10"/>
@@ -1729,8 +1782,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S13" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C14" s="38"/>
       <c r="F14" s="10"/>
       <c r="J14" s="10"/>
@@ -1745,8 +1802,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S14" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C15" s="38"/>
       <c r="F15" s="10"/>
       <c r="J15" s="10"/>
@@ -1761,8 +1822,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S15" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C16" s="38"/>
       <c r="F16" s="10"/>
       <c r="J16" s="10"/>
@@ -1777,8 +1842,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="17" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S16" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C17" s="38"/>
       <c r="F17" s="10"/>
       <c r="J17" s="10"/>
@@ -1793,8 +1862,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="18" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S17" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C18" s="38"/>
       <c r="F18" s="10"/>
       <c r="J18" s="10"/>
@@ -1809,8 +1882,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="19" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S18" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19" s="38"/>
       <c r="F19" s="10"/>
       <c r="J19" s="10"/>
@@ -1825,8 +1902,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="20" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S19" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20" s="38"/>
       <c r="F20" s="10"/>
       <c r="J20" s="10"/>
@@ -1841,8 +1922,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="21" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S20" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21" s="38"/>
       <c r="F21" s="10"/>
       <c r="J21" s="10"/>
@@ -1857,8 +1942,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="22" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S21" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C22" s="38"/>
       <c r="F22" s="10"/>
       <c r="J22" s="10"/>
@@ -1873,8 +1962,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="23" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S22" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C23" s="38"/>
       <c r="F23" s="10"/>
       <c r="J23" s="10"/>
@@ -1889,8 +1982,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="24" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S23" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C24" s="38"/>
       <c r="F24" s="10"/>
       <c r="J24" s="10"/>
@@ -1905,8 +2002,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="25" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S24" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C25" s="38"/>
       <c r="F25" s="10"/>
       <c r="J25" s="10"/>
@@ -1921,8 +2022,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="26" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S25" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C26" s="38"/>
       <c r="F26" s="10"/>
       <c r="J26" s="10"/>
@@ -1937,8 +2042,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="27" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S26" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C27" s="38"/>
       <c r="F27" s="10"/>
       <c r="J27" s="10"/>
@@ -1953,8 +2062,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="28" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S27" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C28" s="38"/>
       <c r="F28" s="10"/>
       <c r="J28" s="10"/>
@@ -1969,8 +2082,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="29" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S28" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C29" s="38"/>
       <c r="F29" s="10"/>
       <c r="J29" s="10"/>
@@ -1985,8 +2102,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="30" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S29" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C30" s="38"/>
       <c r="F30" s="10"/>
       <c r="J30" s="10"/>
@@ -2001,8 +2122,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="31" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S30" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C31" s="38"/>
       <c r="F31" s="10"/>
       <c r="J31" s="10"/>
@@ -2017,8 +2142,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S31" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C32" s="38"/>
       <c r="F32" s="10"/>
       <c r="J32" s="10"/>
@@ -2033,8 +2162,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="33" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S32" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C33" s="38"/>
       <c r="F33" s="10"/>
       <c r="J33" s="10"/>
@@ -2049,8 +2182,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="34" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S33" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C34" s="38"/>
       <c r="F34" s="10"/>
       <c r="J34" s="10"/>
@@ -2065,8 +2202,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="35" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S34" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C35" s="38"/>
       <c r="F35" s="10"/>
       <c r="J35" s="10"/>
@@ -2081,8 +2222,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="36" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S35" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C36" s="38"/>
       <c r="F36" s="10"/>
       <c r="J36" s="10"/>
@@ -2097,8 +2242,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="37" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S36" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C37" s="38"/>
       <c r="F37" s="10"/>
       <c r="J37" s="10"/>
@@ -2113,8 +2262,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="38" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S37" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C38" s="38"/>
       <c r="F38" s="10"/>
       <c r="J38" s="10"/>
@@ -2129,8 +2282,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="39" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S38" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C39" s="38"/>
       <c r="F39" s="10"/>
       <c r="J39" s="10"/>
@@ -2145,8 +2302,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="40" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S39" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C40" s="38"/>
       <c r="F40" s="10"/>
       <c r="J40" s="10"/>
@@ -2161,8 +2322,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="41" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S40" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C41" s="38"/>
       <c r="F41" s="10"/>
       <c r="J41" s="10"/>
@@ -2177,8 +2342,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="42" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S41" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C42" s="38"/>
       <c r="F42" s="10"/>
       <c r="J42" s="10"/>
@@ -2193,8 +2362,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="43" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S42" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C43" s="38"/>
       <c r="F43" s="10"/>
       <c r="J43" s="10"/>
@@ -2209,8 +2382,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="44" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S43" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C44" s="38"/>
       <c r="F44" s="10"/>
       <c r="J44" s="10"/>
@@ -2225,8 +2402,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="45" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S44" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C45" s="38"/>
       <c r="F45" s="10"/>
       <c r="J45" s="10"/>
@@ -2241,8 +2422,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="46" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S45" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C46" s="38"/>
       <c r="F46" s="10"/>
       <c r="J46" s="10"/>
@@ -2257,8 +2442,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="47" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S46" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C47" s="38"/>
       <c r="F47" s="10"/>
       <c r="J47" s="10"/>
@@ -2273,8 +2462,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="48" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S47" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C48" s="38"/>
       <c r="F48" s="10"/>
       <c r="J48" s="10"/>
@@ -2289,8 +2482,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="49" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S48" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C49" s="38"/>
       <c r="F49" s="10"/>
       <c r="J49" s="10"/>
@@ -2305,8 +2502,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="50" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S49" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C50" s="38"/>
       <c r="F50" s="10"/>
       <c r="J50" s="10"/>
@@ -2321,8 +2522,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="51" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S50" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C51" s="38"/>
       <c r="F51" s="10"/>
       <c r="J51" s="10"/>
@@ -2337,8 +2542,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="52" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S51" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C52" s="38"/>
       <c r="F52" s="10"/>
       <c r="J52" s="10"/>
@@ -2353,8 +2562,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="53" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S52" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C53" s="38"/>
       <c r="F53" s="10"/>
       <c r="J53" s="10"/>
@@ -2369,8 +2582,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="54" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S53" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C54" s="38"/>
       <c r="F54" s="10"/>
       <c r="J54" s="10"/>
@@ -2385,8 +2602,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="55" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S54" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C55" s="38"/>
       <c r="F55" s="10"/>
       <c r="J55" s="10"/>
@@ -2401,8 +2622,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="56" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S55" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C56" s="38"/>
       <c r="F56" s="10"/>
       <c r="J56" s="10"/>
@@ -2417,8 +2642,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="57" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S56" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C57" s="38"/>
       <c r="F57" s="10"/>
       <c r="J57" s="10"/>
@@ -2433,8 +2662,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="58" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S57" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C58" s="38"/>
       <c r="F58" s="10"/>
       <c r="J58" s="10"/>
@@ -2449,8 +2682,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="59" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S58" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C59" s="38"/>
       <c r="F59" s="10"/>
       <c r="J59" s="10"/>
@@ -2465,8 +2702,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="60" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S59" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C60" s="38"/>
       <c r="F60" s="10"/>
       <c r="J60" s="10"/>
@@ -2481,8 +2722,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="61" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S60" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C61" s="38"/>
       <c r="F61" s="10"/>
       <c r="J61" s="10"/>
@@ -2497,8 +2742,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="62" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S61" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C62" s="38"/>
       <c r="F62" s="10"/>
       <c r="J62" s="10"/>
@@ -2513,8 +2762,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="63" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S62" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C63" s="38"/>
       <c r="F63" s="10"/>
       <c r="J63" s="10"/>
@@ -2529,8 +2782,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="64" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S63" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C64" s="38"/>
       <c r="F64" s="10"/>
       <c r="J64" s="10"/>
@@ -2545,8 +2802,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="65" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S64" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C65" s="38"/>
       <c r="F65" s="10"/>
       <c r="J65" s="10"/>
@@ -2561,8 +2822,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="66" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S65" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C66" s="38"/>
       <c r="F66" s="10"/>
       <c r="J66" s="10"/>
@@ -2577,8 +2842,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="67" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S66" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C67" s="38"/>
       <c r="F67" s="10"/>
       <c r="J67" s="10"/>
@@ -2593,8 +2862,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="68" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="S67" s="96" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C68" s="38"/>
       <c r="F68" s="10"/>
       <c r="J68" s="10"/>
@@ -2602,15 +2875,19 @@
       <c r="L68" s="10"/>
       <c r="P68" s="51"/>
       <c r="Q68" s="10" t="e">
-        <f t="shared" ref="Q68:Q131" si="2">J68/(H68/100)</f>
+        <f t="shared" ref="Q68:Q131" si="3">J68/(H68/100)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R68" s="9" t="e">
-        <f t="shared" ref="R68:R131" si="3">(P68*1000000)/J68</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="69" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R68:R131" si="4">(P68*1000000)/J68</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S68" s="96" t="e">
+        <f t="shared" ref="S68:S131" si="5">(P68*1000000)/J68</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C69" s="38"/>
       <c r="F69" s="10"/>
       <c r="J69" s="10"/>
@@ -2618,15 +2895,19 @@
       <c r="L69" s="10"/>
       <c r="P69" s="51"/>
       <c r="Q69" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R69" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="70" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S69" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C70" s="38"/>
       <c r="F70" s="10"/>
       <c r="J70" s="10"/>
@@ -2634,15 +2915,19 @@
       <c r="L70" s="10"/>
       <c r="P70" s="51"/>
       <c r="Q70" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R70" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="71" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S70" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C71" s="38"/>
       <c r="F71" s="10"/>
       <c r="J71" s="10"/>
@@ -2650,15 +2935,19 @@
       <c r="L71" s="10"/>
       <c r="P71" s="51"/>
       <c r="Q71" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R71" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="72" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S71" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C72" s="38"/>
       <c r="F72" s="10"/>
       <c r="J72" s="10"/>
@@ -2666,15 +2955,19 @@
       <c r="L72" s="10"/>
       <c r="P72" s="51"/>
       <c r="Q72" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R72" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="73" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S72" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="73" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C73" s="38"/>
       <c r="F73" s="10"/>
       <c r="J73" s="10"/>
@@ -2682,15 +2975,19 @@
       <c r="L73" s="10"/>
       <c r="P73" s="51"/>
       <c r="Q73" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R73" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="74" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S73" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C74" s="38"/>
       <c r="F74" s="10"/>
       <c r="J74" s="10"/>
@@ -2698,15 +2995,19 @@
       <c r="L74" s="10"/>
       <c r="P74" s="51"/>
       <c r="Q74" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R74" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="75" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S74" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C75" s="38"/>
       <c r="F75" s="10"/>
       <c r="J75" s="10"/>
@@ -2714,15 +3015,19 @@
       <c r="L75" s="10"/>
       <c r="P75" s="51"/>
       <c r="Q75" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R75" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="76" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S75" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C76" s="38"/>
       <c r="F76" s="10"/>
       <c r="J76" s="10"/>
@@ -2730,15 +3035,19 @@
       <c r="L76" s="10"/>
       <c r="P76" s="51"/>
       <c r="Q76" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R76" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="77" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S76" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C77" s="38"/>
       <c r="F77" s="10"/>
       <c r="J77" s="10"/>
@@ -2746,15 +3055,19 @@
       <c r="L77" s="10"/>
       <c r="P77" s="51"/>
       <c r="Q77" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R77" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="78" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S77" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C78" s="38"/>
       <c r="F78" s="10"/>
       <c r="J78" s="10"/>
@@ -2762,15 +3075,19 @@
       <c r="L78" s="10"/>
       <c r="P78" s="51"/>
       <c r="Q78" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R78" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="79" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S78" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C79" s="38"/>
       <c r="F79" s="10"/>
       <c r="J79" s="10"/>
@@ -2778,15 +3095,19 @@
       <c r="L79" s="10"/>
       <c r="P79" s="51"/>
       <c r="Q79" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R79" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="80" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S79" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C80" s="38"/>
       <c r="F80" s="10"/>
       <c r="J80" s="10"/>
@@ -2794,15 +3115,19 @@
       <c r="L80" s="10"/>
       <c r="P80" s="51"/>
       <c r="Q80" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R80" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="81" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S80" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C81" s="38"/>
       <c r="F81" s="10"/>
       <c r="J81" s="10"/>
@@ -2810,15 +3135,19 @@
       <c r="L81" s="10"/>
       <c r="P81" s="51"/>
       <c r="Q81" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R81" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="82" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S81" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C82" s="38"/>
       <c r="F82" s="10"/>
       <c r="J82" s="10"/>
@@ -2826,15 +3155,19 @@
       <c r="L82" s="10"/>
       <c r="P82" s="51"/>
       <c r="Q82" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R82" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="83" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S82" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C83" s="38"/>
       <c r="F83" s="10"/>
       <c r="J83" s="10"/>
@@ -2842,15 +3175,19 @@
       <c r="L83" s="10"/>
       <c r="P83" s="51"/>
       <c r="Q83" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R83" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="84" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S83" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C84" s="38"/>
       <c r="F84" s="10"/>
       <c r="J84" s="10"/>
@@ -2858,15 +3195,19 @@
       <c r="L84" s="10"/>
       <c r="P84" s="51"/>
       <c r="Q84" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R84" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="85" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S84" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C85" s="38"/>
       <c r="F85" s="10"/>
       <c r="J85" s="10"/>
@@ -2874,15 +3215,19 @@
       <c r="L85" s="10"/>
       <c r="P85" s="51"/>
       <c r="Q85" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R85" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="86" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S85" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C86" s="38"/>
       <c r="F86" s="10"/>
       <c r="J86" s="10"/>
@@ -2890,15 +3235,19 @@
       <c r="L86" s="10"/>
       <c r="P86" s="51"/>
       <c r="Q86" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R86" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="87" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S86" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C87" s="38"/>
       <c r="F87" s="10"/>
       <c r="J87" s="10"/>
@@ -2906,15 +3255,19 @@
       <c r="L87" s="10"/>
       <c r="P87" s="51"/>
       <c r="Q87" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R87" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="88" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S87" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C88" s="38"/>
       <c r="F88" s="10"/>
       <c r="J88" s="10"/>
@@ -2922,15 +3275,19 @@
       <c r="L88" s="10"/>
       <c r="P88" s="51"/>
       <c r="Q88" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R88" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="89" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S88" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C89" s="38"/>
       <c r="F89" s="10"/>
       <c r="J89" s="10"/>
@@ -2938,15 +3295,19 @@
       <c r="L89" s="10"/>
       <c r="P89" s="51"/>
       <c r="Q89" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R89" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="90" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S89" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C90" s="38"/>
       <c r="F90" s="10"/>
       <c r="J90" s="10"/>
@@ -2954,15 +3315,19 @@
       <c r="L90" s="10"/>
       <c r="P90" s="51"/>
       <c r="Q90" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R90" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="91" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S90" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C91" s="38"/>
       <c r="F91" s="10"/>
       <c r="J91" s="10"/>
@@ -2970,15 +3335,19 @@
       <c r="L91" s="10"/>
       <c r="P91" s="51"/>
       <c r="Q91" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R91" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="92" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S91" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C92" s="38"/>
       <c r="F92" s="10"/>
       <c r="J92" s="10"/>
@@ -2986,15 +3355,19 @@
       <c r="L92" s="10"/>
       <c r="P92" s="51"/>
       <c r="Q92" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R92" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="93" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S92" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C93" s="38"/>
       <c r="F93" s="10"/>
       <c r="J93" s="10"/>
@@ -3002,15 +3375,19 @@
       <c r="L93" s="10"/>
       <c r="P93" s="51"/>
       <c r="Q93" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R93" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="94" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S93" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C94" s="38"/>
       <c r="F94" s="10"/>
       <c r="J94" s="10"/>
@@ -3018,15 +3395,19 @@
       <c r="L94" s="10"/>
       <c r="P94" s="51"/>
       <c r="Q94" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R94" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="95" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S94" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C95" s="38"/>
       <c r="F95" s="10"/>
       <c r="J95" s="10"/>
@@ -3034,15 +3415,19 @@
       <c r="L95" s="10"/>
       <c r="P95" s="51"/>
       <c r="Q95" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R95" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="96" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S95" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C96" s="38"/>
       <c r="F96" s="10"/>
       <c r="J96" s="10"/>
@@ -3050,15 +3435,19 @@
       <c r="L96" s="10"/>
       <c r="P96" s="51"/>
       <c r="Q96" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R96" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="97" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S96" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C97" s="38"/>
       <c r="F97" s="10"/>
       <c r="J97" s="10"/>
@@ -3066,15 +3455,19 @@
       <c r="L97" s="10"/>
       <c r="P97" s="51"/>
       <c r="Q97" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R97" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="98" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S97" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C98" s="38"/>
       <c r="F98" s="10"/>
       <c r="J98" s="10"/>
@@ -3082,15 +3475,19 @@
       <c r="L98" s="10"/>
       <c r="P98" s="51"/>
       <c r="Q98" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R98" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="99" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S98" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C99" s="38"/>
       <c r="F99" s="10"/>
       <c r="J99" s="10"/>
@@ -3098,15 +3495,19 @@
       <c r="L99" s="10"/>
       <c r="P99" s="51"/>
       <c r="Q99" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R99" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="100" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S99" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C100" s="38"/>
       <c r="F100" s="10"/>
       <c r="J100" s="10"/>
@@ -3114,15 +3515,19 @@
       <c r="L100" s="10"/>
       <c r="P100" s="51"/>
       <c r="Q100" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R100" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="101" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S100" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C101" s="38"/>
       <c r="F101" s="10"/>
       <c r="J101" s="10"/>
@@ -3130,15 +3535,19 @@
       <c r="L101" s="10"/>
       <c r="P101" s="51"/>
       <c r="Q101" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R101" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="102" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S101" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="102" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C102" s="38"/>
       <c r="F102" s="10"/>
       <c r="J102" s="10"/>
@@ -3146,15 +3555,19 @@
       <c r="L102" s="10"/>
       <c r="P102" s="51"/>
       <c r="Q102" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R102" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="103" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S102" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="103" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C103" s="38"/>
       <c r="F103" s="10"/>
       <c r="J103" s="10"/>
@@ -3162,15 +3575,19 @@
       <c r="L103" s="10"/>
       <c r="P103" s="51"/>
       <c r="Q103" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R103" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="104" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S103" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="104" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C104" s="38"/>
       <c r="F104" s="10"/>
       <c r="J104" s="10"/>
@@ -3178,15 +3595,19 @@
       <c r="L104" s="10"/>
       <c r="P104" s="51"/>
       <c r="Q104" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R104" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="105" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S104" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="105" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C105" s="38"/>
       <c r="F105" s="10"/>
       <c r="J105" s="10"/>
@@ -3194,15 +3615,19 @@
       <c r="L105" s="10"/>
       <c r="P105" s="51"/>
       <c r="Q105" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R105" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="106" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S105" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="106" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C106" s="38"/>
       <c r="F106" s="10"/>
       <c r="J106" s="10"/>
@@ -3210,15 +3635,19 @@
       <c r="L106" s="10"/>
       <c r="P106" s="51"/>
       <c r="Q106" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R106" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="107" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S106" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="107" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C107" s="38"/>
       <c r="F107" s="10"/>
       <c r="J107" s="10"/>
@@ -3226,15 +3655,19 @@
       <c r="L107" s="10"/>
       <c r="P107" s="51"/>
       <c r="Q107" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R107" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="108" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S107" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="108" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C108" s="38"/>
       <c r="F108" s="10"/>
       <c r="J108" s="10"/>
@@ -3242,15 +3675,19 @@
       <c r="L108" s="10"/>
       <c r="P108" s="51"/>
       <c r="Q108" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R108" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="109" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S108" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="109" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C109" s="38"/>
       <c r="F109" s="10"/>
       <c r="J109" s="10"/>
@@ -3258,15 +3695,19 @@
       <c r="L109" s="10"/>
       <c r="P109" s="51"/>
       <c r="Q109" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R109" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="110" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S109" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="110" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C110" s="38"/>
       <c r="F110" s="10"/>
       <c r="J110" s="10"/>
@@ -3274,15 +3715,19 @@
       <c r="L110" s="10"/>
       <c r="P110" s="51"/>
       <c r="Q110" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R110" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="111" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S110" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="111" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C111" s="38"/>
       <c r="F111" s="10"/>
       <c r="J111" s="10"/>
@@ -3290,15 +3735,19 @@
       <c r="L111" s="10"/>
       <c r="P111" s="51"/>
       <c r="Q111" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R111" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="112" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S111" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="112" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C112" s="38"/>
       <c r="F112" s="10"/>
       <c r="J112" s="10"/>
@@ -3306,15 +3755,19 @@
       <c r="L112" s="10"/>
       <c r="P112" s="51"/>
       <c r="Q112" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R112" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="113" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S112" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="113" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C113" s="38"/>
       <c r="F113" s="10"/>
       <c r="J113" s="10"/>
@@ -3322,15 +3775,19 @@
       <c r="L113" s="10"/>
       <c r="P113" s="51"/>
       <c r="Q113" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R113" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="114" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S113" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="114" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C114" s="38"/>
       <c r="F114" s="10"/>
       <c r="J114" s="10"/>
@@ -3338,15 +3795,19 @@
       <c r="L114" s="10"/>
       <c r="P114" s="51"/>
       <c r="Q114" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R114" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="115" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S114" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="115" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C115" s="38"/>
       <c r="F115" s="10"/>
       <c r="J115" s="10"/>
@@ -3354,15 +3815,19 @@
       <c r="L115" s="10"/>
       <c r="P115" s="51"/>
       <c r="Q115" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R115" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="116" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S115" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="116" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C116" s="38"/>
       <c r="F116" s="10"/>
       <c r="J116" s="10"/>
@@ -3370,15 +3835,19 @@
       <c r="L116" s="10"/>
       <c r="P116" s="51"/>
       <c r="Q116" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R116" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="117" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S116" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="117" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C117" s="38"/>
       <c r="F117" s="10"/>
       <c r="J117" s="10"/>
@@ -3386,15 +3855,19 @@
       <c r="L117" s="10"/>
       <c r="P117" s="51"/>
       <c r="Q117" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R117" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="118" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S117" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="118" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C118" s="38"/>
       <c r="F118" s="10"/>
       <c r="J118" s="10"/>
@@ -3402,15 +3875,19 @@
       <c r="L118" s="10"/>
       <c r="P118" s="51"/>
       <c r="Q118" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R118" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="119" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S118" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="119" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C119" s="38"/>
       <c r="F119" s="10"/>
       <c r="J119" s="10"/>
@@ -3418,15 +3895,19 @@
       <c r="L119" s="10"/>
       <c r="P119" s="51"/>
       <c r="Q119" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R119" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="120" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S119" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="120" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C120" s="38"/>
       <c r="F120" s="10"/>
       <c r="J120" s="10"/>
@@ -3434,15 +3915,19 @@
       <c r="L120" s="10"/>
       <c r="P120" s="51"/>
       <c r="Q120" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R120" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="121" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S120" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="121" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C121" s="38"/>
       <c r="F121" s="10"/>
       <c r="J121" s="10"/>
@@ -3450,15 +3935,19 @@
       <c r="L121" s="10"/>
       <c r="P121" s="51"/>
       <c r="Q121" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R121" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="122" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S121" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="122" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C122" s="38"/>
       <c r="F122" s="10"/>
       <c r="J122" s="10"/>
@@ -3466,15 +3955,19 @@
       <c r="L122" s="10"/>
       <c r="P122" s="51"/>
       <c r="Q122" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R122" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="123" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S122" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="123" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C123" s="38"/>
       <c r="F123" s="10"/>
       <c r="J123" s="10"/>
@@ -3482,15 +3975,19 @@
       <c r="L123" s="10"/>
       <c r="P123" s="51"/>
       <c r="Q123" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R123" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="124" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S123" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="124" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C124" s="38"/>
       <c r="F124" s="10"/>
       <c r="J124" s="10"/>
@@ -3498,15 +3995,19 @@
       <c r="L124" s="10"/>
       <c r="P124" s="51"/>
       <c r="Q124" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R124" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="125" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S124" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="125" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C125" s="38"/>
       <c r="F125" s="10"/>
       <c r="J125" s="10"/>
@@ -3514,15 +4015,19 @@
       <c r="L125" s="10"/>
       <c r="P125" s="51"/>
       <c r="Q125" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R125" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="126" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S125" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="126" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C126" s="38"/>
       <c r="F126" s="10"/>
       <c r="J126" s="10"/>
@@ -3530,15 +4035,19 @@
       <c r="L126" s="10"/>
       <c r="P126" s="51"/>
       <c r="Q126" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R126" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="127" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S126" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="127" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C127" s="38"/>
       <c r="F127" s="10"/>
       <c r="J127" s="10"/>
@@ -3546,15 +4055,19 @@
       <c r="L127" s="10"/>
       <c r="P127" s="51"/>
       <c r="Q127" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R127" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="128" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S127" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="128" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C128" s="38"/>
       <c r="F128" s="10"/>
       <c r="J128" s="10"/>
@@ -3562,15 +4075,19 @@
       <c r="L128" s="10"/>
       <c r="P128" s="51"/>
       <c r="Q128" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R128" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="129" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S128" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="129" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C129" s="38"/>
       <c r="F129" s="10"/>
       <c r="J129" s="10"/>
@@ -3578,15 +4095,19 @@
       <c r="L129" s="10"/>
       <c r="P129" s="51"/>
       <c r="Q129" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R129" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="130" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S129" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="130" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C130" s="38"/>
       <c r="F130" s="10"/>
       <c r="J130" s="10"/>
@@ -3594,15 +4115,19 @@
       <c r="L130" s="10"/>
       <c r="P130" s="51"/>
       <c r="Q130" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R130" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="131" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S130" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="131" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C131" s="38"/>
       <c r="F131" s="10"/>
       <c r="J131" s="10"/>
@@ -3610,15 +4135,19 @@
       <c r="L131" s="10"/>
       <c r="P131" s="51"/>
       <c r="Q131" s="10" t="e">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R131" s="9" t="e">
-        <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="132" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S131" s="96" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="132" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C132" s="38"/>
       <c r="F132" s="10"/>
       <c r="J132" s="10"/>
@@ -3626,15 +4155,19 @@
       <c r="L132" s="10"/>
       <c r="P132" s="51"/>
       <c r="Q132" s="10" t="e">
-        <f t="shared" ref="Q132:Q153" si="4">J132/(H132/100)</f>
+        <f t="shared" ref="Q132:Q153" si="6">J132/(H132/100)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R132" s="9" t="e">
-        <f t="shared" ref="R132:R153" si="5">(P132*1000000)/J132</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="133" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" ref="R132:R153" si="7">(P132*1000000)/J132</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S132" s="96" t="e">
+        <f t="shared" ref="S132:S153" si="8">(P132*1000000)/J132</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="133" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C133" s="38"/>
       <c r="F133" s="10"/>
       <c r="J133" s="10"/>
@@ -3642,15 +4175,19 @@
       <c r="L133" s="10"/>
       <c r="P133" s="51"/>
       <c r="Q133" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R133" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="134" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S133" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="134" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C134" s="38"/>
       <c r="F134" s="10"/>
       <c r="J134" s="10"/>
@@ -3658,15 +4195,19 @@
       <c r="L134" s="10"/>
       <c r="P134" s="51"/>
       <c r="Q134" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R134" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="135" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S134" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="135" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C135" s="38"/>
       <c r="F135" s="10"/>
       <c r="J135" s="10"/>
@@ -3674,15 +4215,19 @@
       <c r="L135" s="10"/>
       <c r="P135" s="51"/>
       <c r="Q135" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R135" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="136" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S135" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="136" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C136" s="38"/>
       <c r="F136" s="10"/>
       <c r="J136" s="10"/>
@@ -3690,15 +4235,19 @@
       <c r="L136" s="10"/>
       <c r="P136" s="51"/>
       <c r="Q136" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R136" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="137" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S136" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="137" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C137" s="38"/>
       <c r="F137" s="10"/>
       <c r="J137" s="10"/>
@@ -3706,15 +4255,19 @@
       <c r="L137" s="10"/>
       <c r="P137" s="51"/>
       <c r="Q137" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R137" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="138" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S137" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="138" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C138" s="38"/>
       <c r="F138" s="10"/>
       <c r="J138" s="10"/>
@@ -3722,15 +4275,19 @@
       <c r="L138" s="10"/>
       <c r="P138" s="51"/>
       <c r="Q138" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R138" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="139" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S138" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="139" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C139" s="38"/>
       <c r="F139" s="10"/>
       <c r="J139" s="10"/>
@@ -3738,15 +4295,19 @@
       <c r="L139" s="10"/>
       <c r="P139" s="51"/>
       <c r="Q139" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R139" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="140" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S139" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="140" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C140" s="38"/>
       <c r="F140" s="10"/>
       <c r="J140" s="10"/>
@@ -3754,15 +4315,19 @@
       <c r="L140" s="10"/>
       <c r="P140" s="51"/>
       <c r="Q140" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R140" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="141" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S140" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="141" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C141" s="38"/>
       <c r="F141" s="10"/>
       <c r="J141" s="10"/>
@@ -3770,15 +4335,19 @@
       <c r="L141" s="10"/>
       <c r="P141" s="51"/>
       <c r="Q141" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R141" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="142" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S141" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="142" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C142" s="38"/>
       <c r="F142" s="10"/>
       <c r="J142" s="10"/>
@@ -3786,15 +4355,19 @@
       <c r="L142" s="10"/>
       <c r="P142" s="51"/>
       <c r="Q142" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R142" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="143" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S142" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="143" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C143" s="38"/>
       <c r="F143" s="10"/>
       <c r="J143" s="10"/>
@@ -3802,15 +4375,19 @@
       <c r="L143" s="10"/>
       <c r="P143" s="51"/>
       <c r="Q143" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R143" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="144" spans="3:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S143" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="144" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C144" s="38"/>
       <c r="F144" s="10"/>
       <c r="J144" s="10"/>
@@ -3818,15 +4395,19 @@
       <c r="L144" s="10"/>
       <c r="P144" s="51"/>
       <c r="Q144" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R144" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S144" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="145" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C145" s="38"/>
       <c r="F145" s="10"/>
       <c r="J145" s="10"/>
@@ -3834,15 +4415,19 @@
       <c r="L145" s="10"/>
       <c r="P145" s="51"/>
       <c r="Q145" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R145" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S145" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="146" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C146" s="38"/>
       <c r="F146" s="10"/>
       <c r="J146" s="10"/>
@@ -3850,15 +4435,19 @@
       <c r="L146" s="10"/>
       <c r="P146" s="51"/>
       <c r="Q146" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R146" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S146" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="147" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C147" s="38"/>
       <c r="F147" s="10"/>
       <c r="J147" s="10"/>
@@ -3866,15 +4455,19 @@
       <c r="L147" s="10"/>
       <c r="P147" s="51"/>
       <c r="Q147" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R147" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S147" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="148" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C148" s="38"/>
       <c r="F148" s="10"/>
       <c r="J148" s="10"/>
@@ -3882,15 +4475,19 @@
       <c r="L148" s="10"/>
       <c r="P148" s="51"/>
       <c r="Q148" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R148" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S148" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="149" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C149" s="38"/>
       <c r="F149" s="10"/>
       <c r="J149" s="10"/>
@@ -3898,15 +4495,19 @@
       <c r="L149" s="10"/>
       <c r="P149" s="51"/>
       <c r="Q149" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R149" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S149" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="150" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C150" s="38"/>
       <c r="F150" s="10"/>
       <c r="J150" s="10"/>
@@ -3914,15 +4515,19 @@
       <c r="L150" s="10"/>
       <c r="P150" s="51"/>
       <c r="Q150" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R150" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S150" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="151" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C151" s="38"/>
       <c r="F151" s="10"/>
       <c r="J151" s="10"/>
@@ -3930,15 +4535,19 @@
       <c r="L151" s="10"/>
       <c r="P151" s="51"/>
       <c r="Q151" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R151" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S151" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="152" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C152" s="38"/>
       <c r="F152" s="10"/>
       <c r="J152" s="10"/>
@@ -3946,15 +4555,19 @@
       <c r="L152" s="10"/>
       <c r="P152" s="51"/>
       <c r="Q152" s="10" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R152" s="9" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S152" s="96" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="153" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A153" s="42"/>
       <c r="B153" s="42"/>
       <c r="C153" s="43"/>
@@ -3972,15 +4585,19 @@
       <c r="O153" s="42"/>
       <c r="P153" s="52"/>
       <c r="Q153" s="72" t="e">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R153" s="50" t="e">
-        <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="S153" s="97" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="154" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C154" s="38"/>
       <c r="F154" s="10"/>
       <c r="J154" s="10"/>
@@ -3988,7 +4605,7 @@
       <c r="L154" s="10"/>
       <c r="P154" s="10"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C155" s="38"/>
       <c r="F155" s="10"/>
       <c r="J155" s="10"/>
@@ -3996,7 +4613,7 @@
       <c r="L155" s="10"/>
       <c r="P155" s="10"/>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C156" s="38"/>
       <c r="F156" s="10"/>
       <c r="J156" s="10"/>
@@ -4004,7 +4621,7 @@
       <c r="L156" s="10"/>
       <c r="P156" s="10"/>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C157" s="38"/>
       <c r="F157" s="10"/>
       <c r="J157" s="10"/>
@@ -4012,21 +4629,21 @@
       <c r="L157" s="10"/>
       <c r="P157" s="10"/>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F158" s="10"/>
       <c r="J158" s="10"/>
       <c r="K158" s="10"/>
       <c r="L158" s="10"/>
       <c r="P158" s="10"/>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F159" s="10"/>
       <c r="J159" s="10"/>
       <c r="K159" s="10"/>
       <c r="L159" s="10"/>
       <c r="P159" s="10"/>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F160" s="10"/>
       <c r="J160" s="10"/>
       <c r="K160" s="10"/>
@@ -5266,13 +5883,13 @@
   <sheetPr>
     <tabColor theme="9" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:N463"/>
+  <dimension ref="A1:O463"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
+      <selection pane="bottomRight" activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5290,9 +5907,10 @@
     <col min="12" max="12" width="20.85546875" customWidth="1"/>
     <col min="13" max="13" width="14.7109375" customWidth="1"/>
     <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C1" s="34" t="s">
         <v>70</v>
       </c>
@@ -5300,19 +5918,20 @@
       <c r="E1" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="F1" s="78" t="s">
+      <c r="F1" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
       <c r="N1" s="8"/>
-    </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="8"/>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="54.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6"/>
       <c r="B2" s="6" t="s">
         <v>10</v>
@@ -5353,8 +5972,11 @@
       <c r="N2" s="71" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2" s="71" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C3" s="38"/>
       <c r="E3" s="10"/>
       <c r="G3" s="10"/>
@@ -5370,8 +5992,12 @@
         <f>(L3*1000000)/M3</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O3" s="9" t="e">
+        <f>(L3*1000000)/G3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" s="38"/>
       <c r="E4" s="10"/>
       <c r="G4" s="10"/>
@@ -5387,8 +6013,12 @@
         <f t="shared" ref="N4:N13" si="1">(L4*1000000)/M4</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4" s="9" t="e">
+        <f t="shared" ref="O4:O13" si="2">(L4*1000000)/G4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="38"/>
       <c r="E5" s="10"/>
       <c r="G5" s="10"/>
@@ -5404,8 +6034,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O5" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="38"/>
       <c r="E6" s="10"/>
       <c r="G6" s="10"/>
@@ -5421,8 +6055,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="38"/>
       <c r="E7" s="10"/>
       <c r="G7" s="10"/>
@@ -5438,8 +6076,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O7" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="38"/>
       <c r="E8" s="10"/>
       <c r="G8" s="10"/>
@@ -5455,8 +6097,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O8" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="38"/>
       <c r="E9" s="10"/>
       <c r="G9" s="10"/>
@@ -5472,8 +6118,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C10" s="38"/>
       <c r="E10" s="10"/>
       <c r="G10" s="10"/>
@@ -5489,8 +6139,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O10" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="38"/>
       <c r="E11" s="10"/>
       <c r="G11" s="10"/>
@@ -5506,8 +6160,12 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O11" s="9" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="38"/>
       <c r="E12" s="10"/>
       <c r="G12" s="10"/>
@@ -5517,8 +6175,9 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="9"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="35"/>
       <c r="B13" s="35" t="s">
         <v>69</v>
@@ -5550,16 +6209,20 @@
         <f t="shared" si="1"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O13" s="37" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E14" s="10"/>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E15" s="10"/>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="E16" s="10"/>
       <c r="I16" s="11"/>
     </row>
@@ -7152,12 +7815,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C1" s="77" t="s">
+      <c r="C1" s="85" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
@@ -10865,10 +11528,10 @@
   <sheetPr>
     <tabColor theme="7" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:K231"/>
+  <dimension ref="A1:L231"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10882,9 +11545,10 @@
     <col min="9" max="9" width="10.85546875" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" customWidth="1"/>
     <col min="11" max="11" width="11.42578125" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
       <c r="B1" s="1" t="s">
         <v>117</v>
@@ -10896,7 +11560,7 @@
       <c r="G1" s="16"/>
       <c r="J1" s="16"/>
     </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="45"/>
       <c r="B2" s="47" t="s">
         <v>10</v>
@@ -10928,8 +11592,11 @@
       <c r="K2" s="49" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3">
         <f>'Region data'!$B3</f>
         <v>0</v>
@@ -10970,8 +11637,12 @@
         <f>'Region data'!$N3</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="9" t="e">
+        <f>'Region data'!$O3</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B4">
         <f>'Region data'!$B4</f>
         <v>0</v>
@@ -11012,8 +11683,12 @@
         <f>'Region data'!$N4</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="9" t="e">
+        <f>'Region data'!$O4</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>'Region data'!$B5</f>
         <v>0</v>
@@ -11054,8 +11729,12 @@
         <f>'Region data'!$N5</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="9" t="e">
+        <f>'Region data'!$O5</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B6">
         <f>'Region data'!$B6</f>
         <v>0</v>
@@ -11096,8 +11775,12 @@
         <f>'Region data'!$N6</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="9" t="e">
+        <f>'Region data'!$O6</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>'Region data'!$B7</f>
         <v>0</v>
@@ -11138,8 +11821,12 @@
         <f>'Region data'!$N7</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="9" t="e">
+        <f>'Region data'!$O7</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8">
         <f>'Region data'!$B8</f>
         <v>0</v>
@@ -11180,8 +11867,12 @@
         <f>'Region data'!$N8</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="9" t="e">
+        <f>'Region data'!$O8</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="22"/>
       <c r="B9">
         <f>'Region data'!$B9</f>
@@ -11223,8 +11914,12 @@
         <f>'Region data'!$N9</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="9" t="e">
+        <f>'Region data'!$O9</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10">
         <f>'Region data'!$B10</f>
@@ -11266,8 +11961,12 @@
         <f>'Region data'!$N10</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="9" t="e">
+        <f>'Region data'!$O10</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11">
         <f>'Region data'!$B11</f>
@@ -11309,8 +12008,12 @@
         <f>'Region data'!$N11</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="9" t="e">
+        <f>'Region data'!$O11</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="22"/>
       <c r="C12" s="38"/>
       <c r="D12" s="10"/>
@@ -11319,8 +12022,9 @@
       <c r="I12" s="10"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="22"/>
       <c r="B13" s="35"/>
       <c r="C13" s="35"/>
@@ -11347,16 +12051,20 @@
         <f>'Region data'!$N13</f>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="37" t="e">
+        <f>'Region data'!$O13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="E14" s="11"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="E15" s="11"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="E16" s="11"/>
     </row>
@@ -12063,86 +12771,86 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="88"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="90"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="90"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="90"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="88"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="90"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="76"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="88"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="90"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="76"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="90"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="76"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="88"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="90"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="76"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="90"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="76"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="90"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="76"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="94"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="80"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
@@ -12180,7 +12888,7 @@
   </sheetPr>
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -12225,86 +12933,86 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="88"/>
-      <c r="D3" s="89"/>
-      <c r="E3" s="88"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="90"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="76"/>
+      <c r="G3" s="77"/>
+      <c r="H3" s="76"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="88"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="90"/>
+      <c r="C4" s="74"/>
+      <c r="D4" s="75"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="77"/>
+      <c r="H4" s="76"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="88"/>
-      <c r="D5" s="89"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="90"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="75"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="76"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="76"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C6" s="88"/>
-      <c r="D6" s="89"/>
-      <c r="E6" s="88"/>
-      <c r="F6" s="90"/>
-      <c r="G6" s="91"/>
-      <c r="H6" s="90"/>
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="76"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="88"/>
-      <c r="D7" s="89"/>
-      <c r="E7" s="88"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="91"/>
-      <c r="H7" s="90"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="75"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="76"/>
+      <c r="G7" s="77"/>
+      <c r="H7" s="76"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="88"/>
-      <c r="F8" s="90"/>
-      <c r="G8" s="91"/>
-      <c r="H8" s="90"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="77"/>
+      <c r="H8" s="76"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="88"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="88"/>
-      <c r="F9" s="90"/>
-      <c r="G9" s="91"/>
-      <c r="H9" s="90"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
+      <c r="H9" s="76"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="88"/>
-      <c r="F10" s="90"/>
-      <c r="G10" s="91"/>
-      <c r="H10" s="90"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="76"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="88"/>
-      <c r="D11" s="89"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="90"/>
-      <c r="G11" s="91"/>
-      <c r="H11" s="90"/>
+      <c r="C11" s="74"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="76"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="42"/>
       <c r="B12" s="42"/>
-      <c r="C12" s="92"/>
-      <c r="D12" s="93"/>
-      <c r="E12" s="92"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="94"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="79"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="80"/>
+      <c r="G12" s="81"/>
+      <c r="H12" s="80"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="69" t="s">
@@ -12557,12 +13265,12 @@
       <c r="E16" s="57"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="83" t="s">
+      <c r="B17" s="91" t="s">
         <v>93</v>
       </c>
-      <c r="C17" s="83"/>
-      <c r="D17" s="83"/>
-      <c r="E17" s="83"/>
+      <c r="C17" s="91"/>
+      <c r="D17" s="91"/>
+      <c r="E17" s="91"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="16" t="s">
@@ -12587,61 +13295,61 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="84" t="str">
+      <c r="B21" s="92" t="str">
         <f>HYPERLINK("https://www.gov.uk/government/statistics/tobacco-bulletin", "(a) 2018/19 figures obtained from the HMRC July 2021 Tobacco Bulletin tables ")</f>
         <v xml:space="preserve">(a) 2018/19 figures obtained from the HMRC July 2021 Tobacco Bulletin tables </v>
       </c>
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
+      <c r="C21" s="93"/>
+      <c r="D21" s="93"/>
+      <c r="E21" s="93"/>
       <c r="F21" s="22"/>
     </row>
     <row r="22" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="79" t="str">
+      <c r="B22" s="87" t="str">
         <f>HYPERLINK("https://ec.europa.eu/taxation_customs/tedb/taxDetails.html?id=4155/1546297200", "(b) European Commission. Weighted Average Price as of 2019/01/01")</f>
         <v>(b) European Commission. Weighted Average Price as of 2019/01/01</v>
       </c>
-      <c r="C22" s="80"/>
-      <c r="D22" s="80"/>
-      <c r="E22" s="80"/>
+      <c r="C22" s="88"/>
+      <c r="D22" s="88"/>
+      <c r="E22" s="88"/>
       <c r="F22" s="22"/>
     </row>
     <row r="23" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="79" t="str">
+      <c r="B23" s="87" t="str">
         <f>HYPERLINK("https://www.gov.uk/government/statistics/tobacco-bulletin/tobacco-duty-rates", "(c) Tobacco duty rates as of December 2018. HMRC Tobacco Bulletin")</f>
         <v>(c) Tobacco duty rates as of December 2018. HMRC Tobacco Bulletin</v>
       </c>
-      <c r="C23" s="80"/>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
       <c r="F23" s="22"/>
     </row>
     <row r="24" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="86" t="s">
+      <c r="B24" s="94" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="86"/>
-      <c r="D24" s="86"/>
-      <c r="E24" s="86"/>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
     </row>
     <row r="25" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="79" t="str">
+      <c r="B25" s="87" t="str">
         <f>HYPERLINK("https://www.gov.uk/government/statistics/measuring-tax-gaps-tables", "(e) 2018/19 illicit consumption obtained from the HMRC Measuring tax gaps tables ")</f>
         <v xml:space="preserve">(e) 2018/19 illicit consumption obtained from the HMRC Measuring tax gaps tables </v>
       </c>
-      <c r="C25" s="80"/>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
+      <c r="C25" s="88"/>
+      <c r="D25" s="88"/>
+      <c r="E25" s="88"/>
       <c r="F25" s="22"/>
     </row>
     <row r="26" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="81" t="str">
+      <c r="B26" s="89" t="str">
         <f>HYPERLINK("https://www.ashscotland.org.uk/media/850413/28-calculating-the-cost-of-smoking-june-2021.pdf", "(f) estimates of illicit tobacco product prices obtained from ASH Scotland ")</f>
         <v xml:space="preserve">(f) estimates of illicit tobacco product prices obtained from ASH Scotland </v>
       </c>
-      <c r="C26" s="82"/>
-      <c r="D26" s="82"/>
-      <c r="E26" s="82"/>
+      <c r="C26" s="90"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="90"/>
       <c r="F26" s="22"/>
     </row>
     <row r="27" spans="2:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -12685,8 +13393,8 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="87"/>
-      <c r="B2" s="87"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="95"/>
       <c r="C2" s="40" t="s">
         <v>72</v>
       </c>

</xml_diff>